<commit_message>
TFS 10823 -  Admin Tool access for Scott potters new job code
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C39952
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" tabRatio="596"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" tabRatio="596" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="345">
   <si>
     <t>SourceID</t>
   </si>
@@ -644,12 +644,6 @@
     <t>Add jobcode WACQ13 in Role_access table(Mark Hackman and Scott Potter)</t>
   </si>
   <si>
-    <t>WACQ13</t>
-  </si>
-  <si>
-    <t>Sr Specialist, Quality (CS)</t>
-  </si>
-  <si>
     <t xml:space="preserve">           ('WISY14','Sr Analyst, Systems',103,'WarningAdmin',0,1),</t>
   </si>
   <si>
@@ -686,12 +680,6 @@
     <t xml:space="preserve">          ('WPPM50','Manager, Program',2,'Supervisor',1) </t>
   </si>
   <si>
-    <t xml:space="preserve">           ('WACQ13','Sr Specialist, Quality (CS)',101,'CoachingAdmin',0,1),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           ('WACQ13','Sr Specialist, Quality (CS)',103,'WarningAdmin',0,1),</t>
-  </si>
-  <si>
     <t xml:space="preserve">           ('WACS60','Sr Manager, Customer Service',105,'SeniorManager',1,1),</t>
   </si>
   <si>
@@ -1025,12 +1013,6 @@
     <t xml:space="preserve">           ('WISY14','Principal Analyst, Systems',107,'ReportWarningAdmin',0,1),</t>
   </si>
   <si>
-    <t xml:space="preserve">           ('WACQ13','Sr Specialist, Quality (CS)',106,'ReportCoachingAdmin',0,1),  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">           ('WACQ13','Sr Specialist, Quality (CS)',107,'ReportWarningAdmin',0,1),</t>
-  </si>
-  <si>
     <t xml:space="preserve">           ('WPSM13','Sr Analyst, Functional',106,'ReportCoachingAdmin',0,1),  </t>
   </si>
   <si>
@@ -1059,6 +1041,27 @@
   </si>
   <si>
     <t>Added rows for job code WPPM11 (New program staff ) in AT_Role_Access tab</t>
+  </si>
+  <si>
+    <t>Added/Updated  rows for job code WPSM12 (Scott.Potter)AT_Role_Access tab</t>
+  </si>
+  <si>
+    <t>WPSM12</t>
+  </si>
+  <si>
+    <t>Analyst, Functional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WPSM12','Analyst, Functional',101,'CoachingAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WPSM12','Analyst, Functional',103,'WarningAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WPSM12',Analyst, Functional',106,'ReportCoachingAdmin',0,1),  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WPSM12','Analyst, Functional',107,'ReportWarningAdmin',0,1),</t>
   </si>
 </sst>
 </file>
@@ -1082,7 +1085,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1092,6 +1095,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1108,13 +1117,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1419,9 +1429,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1531,7 +1543,7 @@
         <v>3027</v>
       </c>
       <c r="E6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1548,7 +1560,7 @@
         <v>5756</v>
       </c>
       <c r="E7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1565,7 +1577,7 @@
         <v>6246</v>
       </c>
       <c r="E8" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1582,7 +1594,7 @@
         <v>5420</v>
       </c>
       <c r="E9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1590,7 +1602,7 @@
         <v>5641</v>
       </c>
       <c r="E10" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1598,7 +1610,7 @@
         <v>5642</v>
       </c>
       <c r="E11" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1615,7 +1627,7 @@
         <v>6591</v>
       </c>
       <c r="E12" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1632,7 +1644,24 @@
         <v>8363</v>
       </c>
       <c r="E13" t="s">
-        <v>343</v>
+        <v>337</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1">
+        <v>43220</v>
+      </c>
+      <c r="C14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14">
+        <v>10823</v>
+      </c>
+      <c r="E14" t="s">
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -1729,7 +1758,7 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1743,7 +1772,7 @@
         <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1757,13 +1786,13 @@
         <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1771,13 +1800,13 @@
         <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1785,13 +1814,13 @@
         <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1799,13 +1828,13 @@
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1813,13 +1842,13 @@
         <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1827,13 +1856,13 @@
         <v>112</v>
       </c>
       <c r="B13" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1841,13 +1870,13 @@
         <v>113</v>
       </c>
       <c r="B14" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1855,13 +1884,13 @@
         <v>114</v>
       </c>
       <c r="B15" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1869,13 +1898,13 @@
         <v>115</v>
       </c>
       <c r="B16" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1883,13 +1912,13 @@
         <v>116</v>
       </c>
       <c r="B17" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1897,13 +1926,13 @@
         <v>117</v>
       </c>
       <c r="B18" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1911,13 +1940,13 @@
         <v>118</v>
       </c>
       <c r="B19" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1925,28 +1954,28 @@
         <v>119</v>
       </c>
       <c r="B20" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F21" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F22" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F23" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -2063,7 +2092,7 @@
         <v>208</v>
       </c>
       <c r="B9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F9" t="s">
         <v>192</v>
@@ -2074,10 +2103,10 @@
         <v>209</v>
       </c>
       <c r="B10" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="F10" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -2085,10 +2114,10 @@
         <v>210</v>
       </c>
       <c r="B11" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F11" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -2096,10 +2125,10 @@
         <v>211</v>
       </c>
       <c r="B12" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F12" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -2107,10 +2136,10 @@
         <v>212</v>
       </c>
       <c r="B13" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F13" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -2118,10 +2147,10 @@
         <v>213</v>
       </c>
       <c r="B14" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F14" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -2129,10 +2158,10 @@
         <v>214</v>
       </c>
       <c r="B15" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F15" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -2140,10 +2169,10 @@
         <v>215</v>
       </c>
       <c r="B16" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F16" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2151,20 +2180,20 @@
         <v>216</v>
       </c>
       <c r="B17" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F17" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F18" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F19" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -2349,7 +2378,7 @@
         <v>209</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2360,7 +2389,7 @@
         <v>210</v>
       </c>
       <c r="F16" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2371,7 +2400,7 @@
         <v>212</v>
       </c>
       <c r="F17" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -2382,7 +2411,7 @@
         <v>213</v>
       </c>
       <c r="F18" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -2393,7 +2422,7 @@
         <v>209</v>
       </c>
       <c r="F19" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -2404,7 +2433,7 @@
         <v>211</v>
       </c>
       <c r="F20" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2415,7 +2444,7 @@
         <v>209</v>
       </c>
       <c r="F21" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -2426,7 +2455,7 @@
         <v>210</v>
       </c>
       <c r="F22" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2437,7 +2466,7 @@
         <v>209</v>
       </c>
       <c r="F23" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -2448,7 +2477,7 @@
         <v>211</v>
       </c>
       <c r="F24" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -2459,7 +2488,7 @@
         <v>209</v>
       </c>
       <c r="F25" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -2470,7 +2499,7 @@
         <v>210</v>
       </c>
       <c r="F26" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -2481,7 +2510,7 @@
         <v>209</v>
       </c>
       <c r="F27" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -2492,7 +2521,7 @@
         <v>211</v>
       </c>
       <c r="F28" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -2503,7 +2532,7 @@
         <v>209</v>
       </c>
       <c r="F29" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -2514,7 +2543,7 @@
         <v>210</v>
       </c>
       <c r="F30" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -2525,7 +2554,7 @@
         <v>209</v>
       </c>
       <c r="F31" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -2536,7 +2565,7 @@
         <v>211</v>
       </c>
       <c r="F32" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -2547,7 +2576,7 @@
         <v>209</v>
       </c>
       <c r="F33" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -2558,7 +2587,7 @@
         <v>210</v>
       </c>
       <c r="F34" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -2569,7 +2598,7 @@
         <v>209</v>
       </c>
       <c r="F35" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -2580,7 +2609,7 @@
         <v>211</v>
       </c>
       <c r="F36" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -2591,7 +2620,7 @@
         <v>209</v>
       </c>
       <c r="F37" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -2602,7 +2631,7 @@
         <v>210</v>
       </c>
       <c r="F38" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -2613,7 +2642,7 @@
         <v>209</v>
       </c>
       <c r="F39" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -2624,7 +2653,7 @@
         <v>211</v>
       </c>
       <c r="F40" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -2635,7 +2664,7 @@
         <v>214</v>
       </c>
       <c r="F41" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -2646,7 +2675,7 @@
         <v>215</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -2657,17 +2686,17 @@
         <v>216</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F44" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F45" s="5" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -3069,7 +3098,7 @@
         <v>197</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3089,7 +3118,7 @@
         <v>197</v>
       </c>
       <c r="B3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3109,7 +3138,7 @@
         <v>197</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -3129,7 +3158,7 @@
         <v>197</v>
       </c>
       <c r="B5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -3149,7 +3178,7 @@
         <v>197</v>
       </c>
       <c r="B6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -3306,10 +3335,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -3326,10 +3355,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -3346,7 +3375,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I16" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.3">
@@ -3361,17 +3390,17 @@
     </row>
     <row r="19" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I20" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I21" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -3622,7 +3651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3658,11 +3687,11 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>205</v>
-      </c>
-      <c r="B2" t="s">
-        <v>206</v>
+      <c r="A2" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>340</v>
       </c>
       <c r="C2">
         <v>101</v>
@@ -3681,11 +3710,11 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>205</v>
-      </c>
-      <c r="B3" t="s">
-        <v>206</v>
+      <c r="A3" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>340</v>
       </c>
       <c r="C3">
         <v>103</v>
@@ -3704,17 +3733,17 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>205</v>
-      </c>
-      <c r="B4" t="s">
-        <v>206</v>
+      <c r="A4" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>340</v>
       </c>
       <c r="C4">
         <v>106</v>
       </c>
       <c r="D4" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -3727,17 +3756,17 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>205</v>
-      </c>
-      <c r="B5" t="s">
-        <v>206</v>
+      <c r="A5" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>340</v>
       </c>
       <c r="C5">
         <v>107</v>
       </c>
       <c r="D5" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3806,7 +3835,7 @@
         <v>105</v>
       </c>
       <c r="D8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -3843,16 +3872,16 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B10" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C10">
         <v>106</v>
       </c>
       <c r="D10" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -3866,16 +3895,16 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B11" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C11">
         <v>107</v>
       </c>
       <c r="D11" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -3889,16 +3918,16 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B12" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C12">
         <v>106</v>
       </c>
       <c r="D12" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -3912,16 +3941,16 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B13" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C13">
         <v>107</v>
       </c>
       <c r="D13" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -3938,7 +3967,7 @@
         <v>197</v>
       </c>
       <c r="B14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C14">
         <v>101</v>
@@ -3961,13 +3990,13 @@
         <v>197</v>
       </c>
       <c r="B15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C15">
         <v>106</v>
       </c>
       <c r="D15" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -3976,7 +4005,7 @@
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -3984,13 +4013,13 @@
         <v>197</v>
       </c>
       <c r="B16" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C16">
         <v>107</v>
       </c>
       <c r="D16" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -3999,7 +4028,7 @@
         <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>219</v>
+        <v>341</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -4007,7 +4036,7 @@
         <v>197</v>
       </c>
       <c r="B17" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C17">
         <v>103</v>
@@ -4022,7 +4051,7 @@
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>220</v>
+        <v>342</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -4045,15 +4074,15 @@
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B19" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C19">
         <v>102</v>
@@ -4068,15 +4097,15 @@
         <v>1</v>
       </c>
       <c r="K19" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B20" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C20">
         <v>101</v>
@@ -4091,15 +4120,15 @@
         <v>1</v>
       </c>
       <c r="K20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B21" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C21">
         <v>103</v>
@@ -4114,21 +4143,21 @@
         <v>1</v>
       </c>
       <c r="K21" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B22" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C22">
         <v>106</v>
       </c>
       <c r="D22" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -4137,21 +4166,21 @@
         <v>1</v>
       </c>
       <c r="K22" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B23" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C23">
         <v>107</v>
       </c>
       <c r="D23" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -4160,21 +4189,21 @@
         <v>1</v>
       </c>
       <c r="K23" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B24" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C24">
         <v>106</v>
       </c>
       <c r="D24" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -4183,21 +4212,21 @@
         <v>1</v>
       </c>
       <c r="K24" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B25" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C25">
         <v>107</v>
       </c>
       <c r="D25" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -4206,21 +4235,21 @@
         <v>1</v>
       </c>
       <c r="K25" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B26" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C26">
         <v>106</v>
       </c>
       <c r="D26" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -4229,21 +4258,21 @@
         <v>1</v>
       </c>
       <c r="K26" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B27" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C27">
         <v>107</v>
       </c>
       <c r="D27" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -4252,21 +4281,21 @@
         <v>1</v>
       </c>
       <c r="K27" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B28" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C28">
         <v>106</v>
       </c>
       <c r="D28" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -4275,21 +4304,21 @@
         <v>1</v>
       </c>
       <c r="K28" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B29" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C29">
         <v>107</v>
       </c>
       <c r="D29" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -4298,7 +4327,7 @@
         <v>1</v>
       </c>
       <c r="K29" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -4321,15 +4350,15 @@
         <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="B31" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C31">
         <v>101</v>
@@ -4344,15 +4373,15 @@
         <v>1</v>
       </c>
       <c r="K31" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="B32" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C32">
         <v>103</v>
@@ -4367,21 +4396,21 @@
         <v>1</v>
       </c>
       <c r="K32" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="B33" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C33">
         <v>106</v>
       </c>
       <c r="D33" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -4390,21 +4419,21 @@
         <v>1</v>
       </c>
       <c r="K33" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="B34" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C34">
         <v>107</v>
       </c>
       <c r="D34" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -4413,42 +4442,42 @@
         <v>1</v>
       </c>
       <c r="K34" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K35" t="s">
-        <v>333</v>
+        <v>344</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K36" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K37" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K38" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K39" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K40" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K41" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 12473 - Access for WPSM14 to the admin tool
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C41106
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" tabRatio="596" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" tabRatio="596"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="AT_Entitlement" sheetId="23" r:id="rId3"/>
     <sheet name="AT_Role_Entitlement_Link" sheetId="28" r:id="rId4"/>
     <sheet name="AT_Action_Reasons" sheetId="24" r:id="rId5"/>
-    <sheet name="AT_Module_Access" sheetId="25" r:id="rId6"/>
+    <sheet name="AT_Module_Access" sheetId="25" state="hidden" r:id="rId6"/>
     <sheet name="AT_Reassign_Status_For_Module" sheetId="26" r:id="rId7"/>
     <sheet name="AT_Role_Access" sheetId="27" r:id="rId8"/>
     <sheet name="Historical_Source" sheetId="6" state="hidden" r:id="rId9"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="347">
   <si>
     <t>SourceID</t>
   </si>
@@ -683,15 +683,9 @@
     <t xml:space="preserve">           ('WACS60','Sr Manager, Customer Service',105,'SeniorManager',1,1),</t>
   </si>
   <si>
-    <t>WPSM13</t>
-  </si>
-  <si>
     <t>Sr Analyst, Functional</t>
   </si>
   <si>
-    <t xml:space="preserve">           ('WPSM13','Sr Analyst, Functional',101,'CoachingAdmin',0,1),</t>
-  </si>
-  <si>
     <t xml:space="preserve">           ('WPPM50','Manager, Program',102,'CoachingUser',1,1),</t>
   </si>
   <si>
@@ -977,9 +971,6 @@
     <t>Principal Engineer, Test</t>
   </si>
   <si>
-    <t xml:space="preserve">           ('WPSM13','Sr Analyst, Functional',103,'WarningAdmin',0,1),</t>
-  </si>
-  <si>
     <t xml:space="preserve">           ('WSTE14','Principal Engineer, Test',106,'ReportCoachingAdmin',0,1),</t>
   </si>
   <si>
@@ -1062,6 +1053,21 @@
   </si>
   <si>
     <t xml:space="preserve">           ('WPSM12','Analyst, Functional',107,'ReportWarningAdmin',0,1),</t>
+  </si>
+  <si>
+    <t>Added rows for job code WPSM14 (Mark Hackman)AT_Role_Access tab</t>
+  </si>
+  <si>
+    <t>Principal Analyst, Functional</t>
+  </si>
+  <si>
+    <t>WPSM14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WPSM14','Principal Analyst, Functional',101,'CoachingAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WPSM14','Principal Analyst, Functional',103,'WarningAdmin',0,1),</t>
   </si>
 </sst>
 </file>
@@ -1085,7 +1091,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1104,6 +1110,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1117,7 +1129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1125,6 +1137,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1429,11 +1443,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1577,7 +1589,7 @@
         <v>6246</v>
       </c>
       <c r="E8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1594,7 +1606,7 @@
         <v>5420</v>
       </c>
       <c r="E9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1602,7 +1614,7 @@
         <v>5641</v>
       </c>
       <c r="E10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1610,7 +1622,7 @@
         <v>5642</v>
       </c>
       <c r="E11" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1627,7 +1639,7 @@
         <v>6591</v>
       </c>
       <c r="E12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1644,7 +1656,7 @@
         <v>8363</v>
       </c>
       <c r="E13" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1661,7 +1673,24 @@
         <v>10823</v>
       </c>
       <c r="E14" t="s">
-        <v>338</v>
+        <v>335</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>11</v>
+      </c>
+      <c r="B15" s="8">
+        <v>43402</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="6">
+        <v>12473</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -1772,7 +1801,7 @@
         <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1786,13 +1815,13 @@
         <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1800,13 +1829,13 @@
         <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1814,13 +1843,13 @@
         <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1828,13 +1857,13 @@
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1842,13 +1871,13 @@
         <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1856,13 +1885,13 @@
         <v>112</v>
       </c>
       <c r="B13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1870,13 +1899,13 @@
         <v>113</v>
       </c>
       <c r="B14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1884,13 +1913,13 @@
         <v>114</v>
       </c>
       <c r="B15" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1898,13 +1927,13 @@
         <v>115</v>
       </c>
       <c r="B16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1912,13 +1941,13 @@
         <v>116</v>
       </c>
       <c r="B17" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1926,13 +1955,13 @@
         <v>117</v>
       </c>
       <c r="B18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1940,13 +1969,13 @@
         <v>118</v>
       </c>
       <c r="B19" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1954,28 +1983,28 @@
         <v>119</v>
       </c>
       <c r="B20" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F21" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F22" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F23" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -2103,10 +2132,10 @@
         <v>209</v>
       </c>
       <c r="B10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -2114,10 +2143,10 @@
         <v>210</v>
       </c>
       <c r="B11" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -2125,10 +2154,10 @@
         <v>211</v>
       </c>
       <c r="B12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F12" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -2136,10 +2165,10 @@
         <v>212</v>
       </c>
       <c r="B13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F13" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -2147,10 +2176,10 @@
         <v>213</v>
       </c>
       <c r="B14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -2158,10 +2187,10 @@
         <v>214</v>
       </c>
       <c r="B15" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F15" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -2169,10 +2198,10 @@
         <v>215</v>
       </c>
       <c r="B16" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F16" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2180,20 +2209,20 @@
         <v>216</v>
       </c>
       <c r="B17" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F17" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F18" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F19" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -2205,7 +2234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
@@ -2378,7 +2407,7 @@
         <v>209</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2389,7 +2418,7 @@
         <v>210</v>
       </c>
       <c r="F16" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2400,7 +2429,7 @@
         <v>212</v>
       </c>
       <c r="F17" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -2411,7 +2440,7 @@
         <v>213</v>
       </c>
       <c r="F18" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -2422,7 +2451,7 @@
         <v>209</v>
       </c>
       <c r="F19" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -2433,7 +2462,7 @@
         <v>211</v>
       </c>
       <c r="F20" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2444,7 +2473,7 @@
         <v>209</v>
       </c>
       <c r="F21" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -2455,7 +2484,7 @@
         <v>210</v>
       </c>
       <c r="F22" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2466,7 +2495,7 @@
         <v>209</v>
       </c>
       <c r="F23" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -2477,7 +2506,7 @@
         <v>211</v>
       </c>
       <c r="F24" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -2488,7 +2517,7 @@
         <v>209</v>
       </c>
       <c r="F25" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -2499,7 +2528,7 @@
         <v>210</v>
       </c>
       <c r="F26" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -2510,7 +2539,7 @@
         <v>209</v>
       </c>
       <c r="F27" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -2521,7 +2550,7 @@
         <v>211</v>
       </c>
       <c r="F28" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -2532,7 +2561,7 @@
         <v>209</v>
       </c>
       <c r="F29" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -2543,7 +2572,7 @@
         <v>210</v>
       </c>
       <c r="F30" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -2554,7 +2583,7 @@
         <v>209</v>
       </c>
       <c r="F31" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -2565,7 +2594,7 @@
         <v>211</v>
       </c>
       <c r="F32" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -2576,7 +2605,7 @@
         <v>209</v>
       </c>
       <c r="F33" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -2587,7 +2616,7 @@
         <v>210</v>
       </c>
       <c r="F34" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -2598,7 +2627,7 @@
         <v>209</v>
       </c>
       <c r="F35" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -2609,7 +2638,7 @@
         <v>211</v>
       </c>
       <c r="F36" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -2620,7 +2649,7 @@
         <v>209</v>
       </c>
       <c r="F37" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -2631,7 +2660,7 @@
         <v>210</v>
       </c>
       <c r="F38" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -2642,7 +2671,7 @@
         <v>209</v>
       </c>
       <c r="F39" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -2653,7 +2682,7 @@
         <v>211</v>
       </c>
       <c r="F40" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -2664,7 +2693,7 @@
         <v>214</v>
       </c>
       <c r="F41" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -2675,7 +2704,7 @@
         <v>215</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -2686,17 +2715,17 @@
         <v>216</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F44" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F45" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -3061,7 +3090,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3651,7 +3682,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:F23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3687,11 +3720,11 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>340</v>
+      <c r="A2" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>337</v>
       </c>
       <c r="C2">
         <v>101</v>
@@ -3710,11 +3743,11 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>340</v>
+      <c r="A3" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>337</v>
       </c>
       <c r="C3">
         <v>103</v>
@@ -3733,17 +3766,17 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>340</v>
+      <c r="A4" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>337</v>
       </c>
       <c r="C4">
         <v>106</v>
       </c>
       <c r="D4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -3756,17 +3789,17 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>340</v>
+      <c r="A5" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>337</v>
       </c>
       <c r="C5">
         <v>107</v>
       </c>
       <c r="D5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3872,16 +3905,16 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B10" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C10">
         <v>106</v>
       </c>
       <c r="D10" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -3895,16 +3928,16 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B11" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C11">
         <v>107</v>
       </c>
       <c r="D11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -3918,16 +3951,16 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B12" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C12">
         <v>106</v>
       </c>
       <c r="D12" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -3941,16 +3974,16 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C13">
         <v>107</v>
       </c>
       <c r="D13" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -3996,7 +4029,7 @@
         <v>106</v>
       </c>
       <c r="D15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -4019,7 +4052,7 @@
         <v>107</v>
       </c>
       <c r="D16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -4028,7 +4061,7 @@
         <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -4051,7 +4084,7 @@
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -4097,113 +4130,113 @@
         <v>1</v>
       </c>
       <c r="K19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="C20" s="6">
+        <v>101</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0</v>
+      </c>
+      <c r="F20" s="6">
+        <v>1</v>
+      </c>
+      <c r="K20" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="B20" t="s">
-        <v>219</v>
-      </c>
-      <c r="C20">
-        <v>101</v>
-      </c>
-      <c r="D20" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="K20" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>218</v>
-      </c>
-      <c r="B21" t="s">
-        <v>219</v>
-      </c>
-      <c r="C21">
+      <c r="C21" s="6">
         <v>103</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
+      <c r="E21" s="6">
+        <v>0</v>
+      </c>
+      <c r="F21" s="6">
         <v>1</v>
       </c>
       <c r="K21" t="s">
-        <v>316</v>
+        <v>346</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>218</v>
-      </c>
-      <c r="B22" t="s">
-        <v>219</v>
-      </c>
-      <c r="C22">
+      <c r="A22" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="C22" s="6">
         <v>106</v>
       </c>
-      <c r="D22" t="s">
-        <v>226</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
+      <c r="D22" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0</v>
+      </c>
+      <c r="F22" s="6">
         <v>1</v>
       </c>
       <c r="K22" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>218</v>
-      </c>
-      <c r="B23" t="s">
-        <v>219</v>
-      </c>
-      <c r="C23">
+      <c r="A23" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="C23" s="6">
         <v>107</v>
       </c>
-      <c r="D23" t="s">
-        <v>227</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
+      <c r="D23" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0</v>
+      </c>
+      <c r="F23" s="6">
         <v>1</v>
       </c>
       <c r="K23" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B24" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C24">
         <v>106</v>
       </c>
       <c r="D24" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -4212,21 +4245,21 @@
         <v>1</v>
       </c>
       <c r="K24" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B25" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C25">
         <v>107</v>
       </c>
       <c r="D25" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -4235,21 +4268,21 @@
         <v>1</v>
       </c>
       <c r="K25" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B26" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C26">
         <v>106</v>
       </c>
       <c r="D26" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -4258,21 +4291,21 @@
         <v>1</v>
       </c>
       <c r="K26" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B27" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C27">
         <v>107</v>
       </c>
       <c r="D27" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -4281,21 +4314,21 @@
         <v>1</v>
       </c>
       <c r="K27" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B28" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C28">
         <v>106</v>
       </c>
       <c r="D28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -4304,21 +4337,21 @@
         <v>1</v>
       </c>
       <c r="K28" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B29" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C29">
         <v>107</v>
       </c>
       <c r="D29" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -4327,7 +4360,7 @@
         <v>1</v>
       </c>
       <c r="K29" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -4350,15 +4383,15 @@
         <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B31" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C31">
         <v>101</v>
@@ -4373,15 +4406,15 @@
         <v>1</v>
       </c>
       <c r="K31" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B32" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C32">
         <v>103</v>
@@ -4396,21 +4429,21 @@
         <v>1</v>
       </c>
       <c r="K32" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B33" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C33">
         <v>106</v>
       </c>
       <c r="D33" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -4419,21 +4452,21 @@
         <v>1</v>
       </c>
       <c r="K33" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B34" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C34">
         <v>107</v>
       </c>
       <c r="D34" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -4442,42 +4475,42 @@
         <v>1</v>
       </c>
       <c r="K34" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K35" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K36" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K37" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K38" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K39" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K40" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K41" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 13333 - Quality Now reporting additional changes
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C42066
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="355">
   <si>
     <t>SourceID</t>
   </si>
@@ -842,9 +842,6 @@
     <t>('Users'),</t>
   </si>
   <si>
-    <t>('User-eCoachingAccessControlList')</t>
-  </si>
-  <si>
     <t>(103,207),</t>
   </si>
   <si>
@@ -935,9 +932,6 @@
     <t>(119,215),</t>
   </si>
   <si>
-    <t>(119,216)</t>
-  </si>
-  <si>
     <t>Added rows for job code WSTE14 (Brian Coughlin)AT_Role_Access tab</t>
   </si>
   <si>
@@ -1068,6 +1062,36 @@
   </si>
   <si>
     <t xml:space="preserve">           ('WPSM14','Principal Analyst, Functional',103,'WarningAdmin',0,1),</t>
+  </si>
+  <si>
+    <t>Added rows to Entitlement and Role entitlement link tables to support new QN Coaching Summary Report</t>
+  </si>
+  <si>
+    <t>Report-RunCoachingSummaryQN</t>
+  </si>
+  <si>
+    <t>('User-eCoachingAccessControlList'),</t>
+  </si>
+  <si>
+    <t>(Report-RunCoachingSummaryQN)</t>
+  </si>
+  <si>
+    <t>(119,216),</t>
+  </si>
+  <si>
+    <t>(106,217),</t>
+  </si>
+  <si>
+    <t>(108,217),</t>
+  </si>
+  <si>
+    <t>(110,217),</t>
+  </si>
+  <si>
+    <t>(112,217),</t>
+  </si>
+  <si>
+    <t>(114,217),</t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1139,6 +1163,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1443,9 +1468,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1639,7 +1666,7 @@
         <v>6591</v>
       </c>
       <c r="E12" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1656,7 +1683,7 @@
         <v>8363</v>
       </c>
       <c r="E13" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1673,24 +1700,41 @@
         <v>10823</v>
       </c>
       <c r="E14" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
         <v>11</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="9">
         <v>43402</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="7">
         <v>12473</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>342</v>
+      <c r="E15" s="7" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>12</v>
+      </c>
+      <c r="B16" s="8">
+        <v>43560</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="6">
+        <v>13333</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -2014,9 +2058,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2216,13 +2262,24 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>217</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>346</v>
+      </c>
       <c r="F18" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F19" t="s">
-        <v>271</v>
+        <v>347</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -2232,10 +2289,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2407,7 +2464,7 @@
         <v>209</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2418,7 +2475,7 @@
         <v>210</v>
       </c>
       <c r="F16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2429,7 +2486,7 @@
         <v>212</v>
       </c>
       <c r="F17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -2440,7 +2497,7 @@
         <v>213</v>
       </c>
       <c r="F18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -2451,7 +2508,7 @@
         <v>209</v>
       </c>
       <c r="F19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -2462,7 +2519,7 @@
         <v>211</v>
       </c>
       <c r="F20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2473,7 +2530,7 @@
         <v>209</v>
       </c>
       <c r="F21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -2484,7 +2541,7 @@
         <v>210</v>
       </c>
       <c r="F22" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2495,7 +2552,7 @@
         <v>209</v>
       </c>
       <c r="F23" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -2506,7 +2563,7 @@
         <v>211</v>
       </c>
       <c r="F24" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -2517,7 +2574,7 @@
         <v>209</v>
       </c>
       <c r="F25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -2528,7 +2585,7 @@
         <v>210</v>
       </c>
       <c r="F26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -2539,7 +2596,7 @@
         <v>209</v>
       </c>
       <c r="F27" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -2550,7 +2607,7 @@
         <v>211</v>
       </c>
       <c r="F28" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -2561,7 +2618,7 @@
         <v>209</v>
       </c>
       <c r="F29" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -2572,7 +2629,7 @@
         <v>210</v>
       </c>
       <c r="F30" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -2583,7 +2640,7 @@
         <v>209</v>
       </c>
       <c r="F31" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -2594,7 +2651,7 @@
         <v>211</v>
       </c>
       <c r="F32" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -2605,7 +2662,7 @@
         <v>209</v>
       </c>
       <c r="F33" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -2616,7 +2673,7 @@
         <v>210</v>
       </c>
       <c r="F34" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -2627,7 +2684,7 @@
         <v>209</v>
       </c>
       <c r="F35" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -2638,7 +2695,7 @@
         <v>211</v>
       </c>
       <c r="F36" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -2649,7 +2706,7 @@
         <v>209</v>
       </c>
       <c r="F37" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -2660,7 +2717,7 @@
         <v>210</v>
       </c>
       <c r="F38" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -2671,7 +2728,7 @@
         <v>209</v>
       </c>
       <c r="F39" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -2682,7 +2739,7 @@
         <v>211</v>
       </c>
       <c r="F40" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -2693,7 +2750,7 @@
         <v>214</v>
       </c>
       <c r="F41" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -2704,7 +2761,7 @@
         <v>215</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -2715,17 +2772,83 @@
         <v>216</v>
       </c>
       <c r="F43" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="6">
+        <v>106</v>
+      </c>
+      <c r="B44" s="6">
+        <v>217</v>
+      </c>
+      <c r="F44" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F44" t="s">
-        <v>301</v>
-      </c>
-    </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="6">
+        <v>108</v>
+      </c>
+      <c r="B45" s="6">
+        <v>217</v>
+      </c>
       <c r="F45" s="5" t="s">
-        <v>302</v>
+        <v>349</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="6">
+        <v>110</v>
+      </c>
+      <c r="B46" s="6">
+        <v>217</v>
+      </c>
+      <c r="F46" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="6">
+        <v>112</v>
+      </c>
+      <c r="B47" s="6">
+        <v>217</v>
+      </c>
+      <c r="F47" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="6">
+        <v>114</v>
+      </c>
+      <c r="B48" s="6">
+        <v>217</v>
+      </c>
+      <c r="F48" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="6">
+        <v>116</v>
+      </c>
+      <c r="B49" s="6">
+        <v>217</v>
+      </c>
+      <c r="F49" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F50" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F51" t="s">
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -3721,10 +3844,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C2">
         <v>101</v>
@@ -3744,10 +3867,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C3">
         <v>103</v>
@@ -3767,10 +3890,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C4">
         <v>106</v>
@@ -3790,10 +3913,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C5">
         <v>107</v>
@@ -3905,10 +4028,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B10" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C10">
         <v>106</v>
@@ -3928,10 +4051,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C11">
         <v>107</v>
@@ -3951,10 +4074,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C12">
         <v>106</v>
@@ -3974,10 +4097,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B13" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C13">
         <v>107</v>
@@ -4061,7 +4184,7 @@
         <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -4084,7 +4207,7 @@
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -4135,10 +4258,10 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C20" s="6">
         <v>101</v>
@@ -4153,12 +4276,12 @@
         <v>1</v>
       </c>
       <c r="K20" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>218</v>
@@ -4176,15 +4299,15 @@
         <v>1</v>
       </c>
       <c r="K21" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C22" s="6">
         <v>106</v>
@@ -4199,15 +4322,15 @@
         <v>1</v>
       </c>
       <c r="K22" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C23" s="6">
         <v>107</v>
@@ -4222,15 +4345,15 @@
         <v>1</v>
       </c>
       <c r="K23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B24" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C24">
         <v>106</v>
@@ -4245,15 +4368,15 @@
         <v>1</v>
       </c>
       <c r="K24" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B25" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C25">
         <v>107</v>
@@ -4268,15 +4391,15 @@
         <v>1</v>
       </c>
       <c r="K25" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B26" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C26">
         <v>106</v>
@@ -4291,15 +4414,15 @@
         <v>1</v>
       </c>
       <c r="K26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B27" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C27">
         <v>107</v>
@@ -4314,15 +4437,15 @@
         <v>1</v>
       </c>
       <c r="K27" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B28" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C28">
         <v>106</v>
@@ -4337,15 +4460,15 @@
         <v>1</v>
       </c>
       <c r="K28" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B29" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C29">
         <v>107</v>
@@ -4360,7 +4483,7 @@
         <v>1</v>
       </c>
       <c r="K29" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -4383,15 +4506,15 @@
         <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B31" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C31">
         <v>101</v>
@@ -4406,15 +4529,15 @@
         <v>1</v>
       </c>
       <c r="K31" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B32" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C32">
         <v>103</v>
@@ -4429,15 +4552,15 @@
         <v>1</v>
       </c>
       <c r="K32" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B33" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C33">
         <v>106</v>
@@ -4452,15 +4575,15 @@
         <v>1</v>
       </c>
       <c r="K33" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B34" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C34">
         <v>107</v>
@@ -4475,42 +4598,42 @@
         <v>1</v>
       </c>
       <c r="K34" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K35" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K36" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K37" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K38" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K39" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K40" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K41" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 13644 – Incorporate a follow-up process for eCoaching submissions
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C43285
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cms\eCoaching_V2\Design\DD\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OmniCloud\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="357">
   <si>
     <t>SourceID</t>
   </si>
@@ -518,12 +518,6 @@
     <t xml:space="preserve">            (5,'Training',5, 'Pending Manager Review',1),</t>
   </si>
   <si>
-    <t xml:space="preserve">            (5,'Training',6, 'Pending Supervisor Review',1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            </t>
-  </si>
-  <si>
     <t xml:space="preserve">           ,[Status] </t>
   </si>
   <si>
@@ -1092,6 +1086,18 @@
   </si>
   <si>
     <t>(114,217),</t>
+  </si>
+  <si>
+    <t>Pending Follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            (1, 'CSR', 10, 'Pending Follow-up', 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            (5,'Training',6, 'Pending Supervisor Review',1),</t>
+  </si>
+  <si>
+    <t>Incorporate a follow-up process for eCoaching submissions. Added new status in AT_Reassign_Status_For_Module</t>
   </si>
 </sst>
 </file>
@@ -1468,10 +1474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1531,7 +1537,7 @@
         <v>1709</v>
       </c>
       <c r="E3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1548,7 +1554,7 @@
         <v>3416</v>
       </c>
       <c r="E4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1565,7 +1571,7 @@
         <v>3877</v>
       </c>
       <c r="E5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1582,7 +1588,7 @@
         <v>3027</v>
       </c>
       <c r="E6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1599,7 +1605,7 @@
         <v>5756</v>
       </c>
       <c r="E7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1616,7 +1622,7 @@
         <v>6246</v>
       </c>
       <c r="E8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1633,7 +1639,7 @@
         <v>5420</v>
       </c>
       <c r="E9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1641,7 +1647,7 @@
         <v>5641</v>
       </c>
       <c r="E10" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1649,7 +1655,7 @@
         <v>5642</v>
       </c>
       <c r="E11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1666,7 +1672,7 @@
         <v>6591</v>
       </c>
       <c r="E12" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1683,7 +1689,7 @@
         <v>8363</v>
       </c>
       <c r="E13" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1700,7 +1706,7 @@
         <v>10823</v>
       </c>
       <c r="E14" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -1717,24 +1723,41 @@
         <v>12473</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="6">
+      <c r="A16" s="7">
         <v>12</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="9">
         <v>43560</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="7">
         <v>13333</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>345</v>
+      <c r="E16" s="7" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>13</v>
+      </c>
+      <c r="B17" s="8">
+        <v>43714</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="6">
+        <v>13644</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -1831,7 +1854,7 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1845,7 +1868,7 @@
         <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1859,13 +1882,13 @@
         <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1873,13 +1896,13 @@
         <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1887,13 +1910,13 @@
         <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1901,13 +1924,13 @@
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1915,13 +1938,13 @@
         <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1929,13 +1952,13 @@
         <v>112</v>
       </c>
       <c r="B13" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1943,13 +1966,13 @@
         <v>113</v>
       </c>
       <c r="B14" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1957,13 +1980,13 @@
         <v>114</v>
       </c>
       <c r="B15" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1971,13 +1994,13 @@
         <v>115</v>
       </c>
       <c r="B16" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1985,13 +2008,13 @@
         <v>116</v>
       </c>
       <c r="B17" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1999,13 +2022,13 @@
         <v>117</v>
       </c>
       <c r="B18" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -2013,13 +2036,13 @@
         <v>118</v>
       </c>
       <c r="B19" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -2027,28 +2050,28 @@
         <v>119</v>
       </c>
       <c r="B20" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F21" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F22" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F23" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -2104,7 +2127,7 @@
         <v>113</v>
       </c>
       <c r="H3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -2145,7 +2168,7 @@
         <v>206</v>
       </c>
       <c r="B7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F7" t="s">
         <v>123</v>
@@ -2156,10 +2179,10 @@
         <v>207</v>
       </c>
       <c r="B8" t="s">
+        <v>187</v>
+      </c>
+      <c r="F8" t="s">
         <v>189</v>
-      </c>
-      <c r="F8" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -2167,10 +2190,10 @@
         <v>208</v>
       </c>
       <c r="B9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -2178,10 +2201,10 @@
         <v>209</v>
       </c>
       <c r="B10" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -2189,10 +2212,10 @@
         <v>210</v>
       </c>
       <c r="B11" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -2200,10 +2223,10 @@
         <v>211</v>
       </c>
       <c r="B12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -2211,10 +2234,10 @@
         <v>212</v>
       </c>
       <c r="B13" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -2222,10 +2245,10 @@
         <v>213</v>
       </c>
       <c r="B14" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F14" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -2233,10 +2256,10 @@
         <v>214</v>
       </c>
       <c r="B15" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F15" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -2244,10 +2267,10 @@
         <v>215</v>
       </c>
       <c r="B16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F16" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2255,10 +2278,10 @@
         <v>216</v>
       </c>
       <c r="B17" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F17" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -2266,20 +2289,20 @@
         <v>217</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F18" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F19" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F20" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -2310,7 +2333,7 @@
         <v>86</v>
       </c>
       <c r="F1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2321,7 +2344,7 @@
         <v>201</v>
       </c>
       <c r="F2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2343,7 +2366,7 @@
         <v>203</v>
       </c>
       <c r="F4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -2354,7 +2377,7 @@
         <v>204</v>
       </c>
       <c r="F5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2365,7 +2388,7 @@
         <v>206</v>
       </c>
       <c r="F6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2376,7 +2399,7 @@
         <v>201</v>
       </c>
       <c r="F7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2387,7 +2410,7 @@
         <v>202</v>
       </c>
       <c r="F8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -2398,7 +2421,7 @@
         <v>204</v>
       </c>
       <c r="F9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -2409,7 +2432,7 @@
         <v>201</v>
       </c>
       <c r="F10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2420,7 +2443,7 @@
         <v>203</v>
       </c>
       <c r="F11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -2431,7 +2454,7 @@
         <v>205</v>
       </c>
       <c r="F12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2442,7 +2465,7 @@
         <v>207</v>
       </c>
       <c r="F13" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -2453,7 +2476,7 @@
         <v>208</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -2464,7 +2487,7 @@
         <v>209</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2475,7 +2498,7 @@
         <v>210</v>
       </c>
       <c r="F16" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2486,7 +2509,7 @@
         <v>212</v>
       </c>
       <c r="F17" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -2497,7 +2520,7 @@
         <v>213</v>
       </c>
       <c r="F18" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -2508,7 +2531,7 @@
         <v>209</v>
       </c>
       <c r="F19" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -2519,7 +2542,7 @@
         <v>211</v>
       </c>
       <c r="F20" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2530,7 +2553,7 @@
         <v>209</v>
       </c>
       <c r="F21" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -2541,7 +2564,7 @@
         <v>210</v>
       </c>
       <c r="F22" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2552,7 +2575,7 @@
         <v>209</v>
       </c>
       <c r="F23" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -2563,7 +2586,7 @@
         <v>211</v>
       </c>
       <c r="F24" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -2574,7 +2597,7 @@
         <v>209</v>
       </c>
       <c r="F25" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -2585,7 +2608,7 @@
         <v>210</v>
       </c>
       <c r="F26" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -2596,7 +2619,7 @@
         <v>209</v>
       </c>
       <c r="F27" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -2607,7 +2630,7 @@
         <v>211</v>
       </c>
       <c r="F28" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -2618,7 +2641,7 @@
         <v>209</v>
       </c>
       <c r="F29" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -2629,7 +2652,7 @@
         <v>210</v>
       </c>
       <c r="F30" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -2640,7 +2663,7 @@
         <v>209</v>
       </c>
       <c r="F31" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -2651,7 +2674,7 @@
         <v>211</v>
       </c>
       <c r="F32" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -2662,7 +2685,7 @@
         <v>209</v>
       </c>
       <c r="F33" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -2673,7 +2696,7 @@
         <v>210</v>
       </c>
       <c r="F34" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -2684,7 +2707,7 @@
         <v>209</v>
       </c>
       <c r="F35" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -2695,7 +2718,7 @@
         <v>211</v>
       </c>
       <c r="F36" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -2706,7 +2729,7 @@
         <v>209</v>
       </c>
       <c r="F37" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -2717,7 +2740,7 @@
         <v>210</v>
       </c>
       <c r="F38" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -2728,7 +2751,7 @@
         <v>209</v>
       </c>
       <c r="F39" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -2739,7 +2762,7 @@
         <v>211</v>
       </c>
       <c r="F40" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -2750,7 +2773,7 @@
         <v>214</v>
       </c>
       <c r="F41" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -2761,7 +2784,7 @@
         <v>215</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -2772,7 +2795,7 @@
         <v>216</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -2783,7 +2806,7 @@
         <v>217</v>
       </c>
       <c r="F44" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -2794,7 +2817,7 @@
         <v>217</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -2805,7 +2828,7 @@
         <v>217</v>
       </c>
       <c r="F46" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -2816,7 +2839,7 @@
         <v>217</v>
       </c>
       <c r="F47" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -2827,7 +2850,7 @@
         <v>217</v>
       </c>
       <c r="F48" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -2838,17 +2861,17 @@
         <v>217</v>
       </c>
       <c r="F49" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F50" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F51" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -3249,10 +3272,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3269,10 +3292,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3289,10 +3312,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -3309,10 +3332,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -3329,10 +3352,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -3384,7 +3407,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -3404,7 +3427,7 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -3424,7 +3447,7 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -3444,7 +3467,7 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -3464,7 +3487,7 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -3489,10 +3512,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -3509,10 +3532,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -3524,12 +3547,12 @@
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.3">
@@ -3544,17 +3567,17 @@
     </row>
     <row r="19" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I19" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I20" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I21" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -3566,7 +3589,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3708,7 +3733,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -3752,6 +3777,21 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>1</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="6">
+        <v>10</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1</v>
+      </c>
       <c r="J10" t="s">
         <v>156</v>
       </c>
@@ -3788,12 +3828,12 @@
     </row>
     <row r="17" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J17" t="s">
-        <v>163</v>
+        <v>355</v>
       </c>
     </row>
     <row r="18" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J18" t="s">
-        <v>164</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -3833,21 +3873,21 @@
         <v>80</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>53</v>
       </c>
       <c r="K1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C2">
         <v>101</v>
@@ -3867,10 +3907,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C3">
         <v>103</v>
@@ -3890,16 +3930,16 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C4">
         <v>106</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -3908,21 +3948,21 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C5">
         <v>107</v>
       </c>
       <c r="D5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3931,7 +3971,7 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -3954,7 +3994,7 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -3991,7 +4031,7 @@
         <v>105</v>
       </c>
       <c r="D8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -4023,21 +4063,21 @@
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C10">
         <v>106</v>
       </c>
       <c r="D10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -4046,21 +4086,21 @@
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B11" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C11">
         <v>107</v>
       </c>
       <c r="D11" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -4069,21 +4109,21 @@
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C12">
         <v>106</v>
       </c>
       <c r="D12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -4092,21 +4132,21 @@
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B13" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C13">
         <v>107</v>
       </c>
       <c r="D13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -4115,15 +4155,15 @@
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C14">
         <v>101</v>
@@ -4138,21 +4178,21 @@
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C15">
         <v>106</v>
       </c>
       <c r="D15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -4161,21 +4201,21 @@
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B16" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C16">
         <v>107</v>
       </c>
       <c r="D16" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -4184,15 +4224,15 @@
         <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B17" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C17">
         <v>103</v>
@@ -4207,7 +4247,7 @@
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -4230,15 +4270,15 @@
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C19">
         <v>102</v>
@@ -4253,15 +4293,15 @@
         <v>1</v>
       </c>
       <c r="K19" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C20" s="6">
         <v>101</v>
@@ -4276,15 +4316,15 @@
         <v>1</v>
       </c>
       <c r="K20" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C21" s="6">
         <v>103</v>
@@ -4299,21 +4339,21 @@
         <v>1</v>
       </c>
       <c r="K21" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C22" s="6">
         <v>106</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E22" s="6">
         <v>0</v>
@@ -4322,21 +4362,21 @@
         <v>1</v>
       </c>
       <c r="K22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C23" s="6">
         <v>107</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E23" s="6">
         <v>0</v>
@@ -4345,21 +4385,21 @@
         <v>1</v>
       </c>
       <c r="K23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B24" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C24">
         <v>106</v>
       </c>
       <c r="D24" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -4368,21 +4408,21 @@
         <v>1</v>
       </c>
       <c r="K24" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B25" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C25">
         <v>107</v>
       </c>
       <c r="D25" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -4391,21 +4431,21 @@
         <v>1</v>
       </c>
       <c r="K25" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B26" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C26">
         <v>106</v>
       </c>
       <c r="D26" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -4414,21 +4454,21 @@
         <v>1</v>
       </c>
       <c r="K26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B27" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C27">
         <v>107</v>
       </c>
       <c r="D27" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -4437,21 +4477,21 @@
         <v>1</v>
       </c>
       <c r="K27" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B28" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C28">
         <v>106</v>
       </c>
       <c r="D28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -4460,21 +4500,21 @@
         <v>1</v>
       </c>
       <c r="K28" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B29" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C29">
         <v>107</v>
       </c>
       <c r="D29" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -4483,7 +4523,7 @@
         <v>1</v>
       </c>
       <c r="K29" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -4506,15 +4546,15 @@
         <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B31" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C31">
         <v>101</v>
@@ -4529,15 +4569,15 @@
         <v>1</v>
       </c>
       <c r="K31" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B32" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C32">
         <v>103</v>
@@ -4552,21 +4592,21 @@
         <v>1</v>
       </c>
       <c r="K32" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B33" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C33">
         <v>106</v>
       </c>
       <c r="D33" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -4575,21 +4615,21 @@
         <v>1</v>
       </c>
       <c r="K33" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B34" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C34">
         <v>107</v>
       </c>
       <c r="D34" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -4598,42 +4638,42 @@
         <v>1</v>
       </c>
       <c r="K34" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K35" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K36" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K37" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K38" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K39" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K40" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K41" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 22187 - Quality Now workflow Enhancement and TFS 23051 - New Coaching Reason for Quality
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C50548
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\omnicloud\eCoaching_V2\Design\DD\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OmniCloud\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40A8249-9ABC-4041-B641-89E0E79C0050}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840" tabRatio="596"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="596" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="200">
   <si>
     <t>SourceID</t>
   </si>
@@ -621,12 +622,21 @@
   </si>
   <si>
     <t>Sr Manager access control tables cleanup</t>
+  </si>
+  <si>
+    <t>Added rows to AT_Reassign_Status_For_Module</t>
+  </si>
+  <si>
+    <t>Pending Follow-up Preparation</t>
+  </si>
+  <si>
+    <t>Pending Follow-up Coaching</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -786,6 +796,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -821,6 +848,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -996,23 +1040,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.68359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="144.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.83984375" customWidth="1"/>
+    <col min="5" max="5" width="144.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>68</v>
       </c>
@@ -1029,7 +1073,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1046,7 +1090,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
@@ -1063,7 +1107,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1080,7 +1124,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1097,7 +1141,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1114,7 +1158,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1131,7 +1175,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1148,7 +1192,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1165,7 +1209,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D10">
         <v>5641</v>
       </c>
@@ -1173,7 +1217,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D11">
         <v>5642</v>
       </c>
@@ -1181,7 +1225,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1198,7 +1242,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1215,7 +1259,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1232,7 +1276,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7">
         <v>11</v>
       </c>
@@ -1249,7 +1293,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="7">
         <v>12</v>
       </c>
@@ -1266,7 +1310,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="7">
         <v>13</v>
       </c>
@@ -1283,21 +1327,38 @@
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+    <row r="18" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="7">
         <v>14</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="9">
         <v>44049</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="7">
         <v>18019</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="7" t="s">
         <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="6">
+        <v>15</v>
+      </c>
+      <c r="B19" s="8">
+        <v>44454</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="6">
+        <v>22187</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -1307,21 +1368,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.41796875" customWidth="1"/>
+    <col min="3" max="3" width="11.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>79</v>
       </c>
@@ -1332,7 +1393,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>101</v>
       </c>
@@ -1343,7 +1404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>102</v>
       </c>
@@ -1354,7 +1415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>103</v>
       </c>
@@ -1365,7 +1426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>104</v>
       </c>
@@ -1376,7 +1437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>106</v>
       </c>
@@ -1387,7 +1448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>107</v>
       </c>
@@ -1398,7 +1459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>108</v>
       </c>
@@ -1409,7 +1470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>109</v>
       </c>
@@ -1420,7 +1481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>110</v>
       </c>
@@ -1431,7 +1492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>111</v>
       </c>
@@ -1442,7 +1503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>112</v>
       </c>
@@ -1453,7 +1514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>113</v>
       </c>
@@ -1464,7 +1525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>114</v>
       </c>
@@ -1475,7 +1536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>115</v>
       </c>
@@ -1486,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>116</v>
       </c>
@@ -1497,7 +1558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>117</v>
       </c>
@@ -1508,7 +1569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>118</v>
       </c>
@@ -1519,7 +1580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>119</v>
       </c>
@@ -1536,21 +1597,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="57.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.26171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="57.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>86</v>
       </c>
@@ -1558,7 +1619,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>201</v>
       </c>
@@ -1566,7 +1627,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>202</v>
       </c>
@@ -1577,7 +1638,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>203</v>
       </c>
@@ -1585,7 +1646,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>204</v>
       </c>
@@ -1593,7 +1654,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>205</v>
       </c>
@@ -1601,7 +1662,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>206</v>
       </c>
@@ -1609,7 +1670,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>207</v>
       </c>
@@ -1617,7 +1678,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>209</v>
       </c>
@@ -1625,7 +1686,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>210</v>
       </c>
@@ -1633,7 +1694,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>211</v>
       </c>
@@ -1641,7 +1702,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>212</v>
       </c>
@@ -1649,7 +1710,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>213</v>
       </c>
@@ -1657,7 +1718,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>214</v>
       </c>
@@ -1665,7 +1726,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>215</v>
       </c>
@@ -1673,7 +1734,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>216</v>
       </c>
@@ -1681,7 +1742,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="7">
         <v>217</v>
       </c>
@@ -1695,21 +1756,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="62.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.41796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="62.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>79</v>
       </c>
@@ -1717,7 +1778,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>101</v>
       </c>
@@ -1725,7 +1786,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>101</v>
       </c>
@@ -1733,7 +1794,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>101</v>
       </c>
@@ -1741,7 +1802,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>101</v>
       </c>
@@ -1749,7 +1810,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>101</v>
       </c>
@@ -1757,7 +1818,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>102</v>
       </c>
@@ -1765,7 +1826,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>102</v>
       </c>
@@ -1773,7 +1834,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>102</v>
       </c>
@@ -1781,7 +1842,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>103</v>
       </c>
@@ -1789,7 +1850,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>103</v>
       </c>
@@ -1797,7 +1858,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>103</v>
       </c>
@@ -1805,7 +1866,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>103</v>
       </c>
@@ -1813,7 +1874,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>106</v>
       </c>
@@ -1822,7 +1883,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>106</v>
       </c>
@@ -1830,7 +1891,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>106</v>
       </c>
@@ -1838,7 +1899,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>106</v>
       </c>
@@ -1846,7 +1907,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>107</v>
       </c>
@@ -1854,7 +1915,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>107</v>
       </c>
@@ -1862,7 +1923,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>108</v>
       </c>
@@ -1870,7 +1931,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>108</v>
       </c>
@@ -1878,7 +1939,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>109</v>
       </c>
@@ -1886,7 +1947,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>109</v>
       </c>
@@ -1894,7 +1955,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>110</v>
       </c>
@@ -1902,7 +1963,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>110</v>
       </c>
@@ -1910,7 +1971,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>111</v>
       </c>
@@ -1918,7 +1979,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>111</v>
       </c>
@@ -1926,7 +1987,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>112</v>
       </c>
@@ -1934,7 +1995,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>112</v>
       </c>
@@ -1942,7 +2003,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>113</v>
       </c>
@@ -1950,7 +2011,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>113</v>
       </c>
@@ -1958,7 +2019,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>114</v>
       </c>
@@ -1966,7 +2027,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>114</v>
       </c>
@@ -1974,7 +2035,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>115</v>
       </c>
@@ -1982,7 +2043,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>115</v>
       </c>
@@ -1990,7 +2051,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>116</v>
       </c>
@@ -1998,7 +2059,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>116</v>
       </c>
@@ -2006,7 +2067,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <v>117</v>
       </c>
@@ -2014,7 +2075,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <v>117</v>
       </c>
@@ -2022,7 +2083,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>118</v>
       </c>
@@ -2030,7 +2091,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>119</v>
       </c>
@@ -2039,7 +2100,7 @@
       </c>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>119</v>
       </c>
@@ -2048,7 +2109,7 @@
       </c>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="7">
         <v>106</v>
       </c>
@@ -2056,7 +2117,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="7">
         <v>108</v>
       </c>
@@ -2065,7 +2126,7 @@
       </c>
       <c r="F44" s="5"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="7">
         <v>110</v>
       </c>
@@ -2073,7 +2134,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="7">
         <v>112</v>
       </c>
@@ -2081,7 +2142,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="7">
         <v>114</v>
       </c>
@@ -2089,7 +2150,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="7">
         <v>116</v>
       </c>
@@ -2098,32 +2159,32 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A50"/>
+  <autoFilter ref="A1:A50" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.26171875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.41796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.68359375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.26171875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>93</v>
       </c>
@@ -2149,7 +2210,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2175,7 +2236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2201,7 +2262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2227,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2253,7 +2314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2279,7 +2340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2305,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2331,7 +2392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2357,7 +2418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2389,24 +2450,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.41796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="101.42578125" customWidth="1"/>
+    <col min="9" max="9" width="101.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>106</v>
       </c>
@@ -2426,7 +2487,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -2446,7 +2507,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -2466,7 +2527,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>129</v>
       </c>
@@ -2486,7 +2547,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -2506,7 +2567,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>129</v>
       </c>
@@ -2526,7 +2587,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -2546,7 +2607,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -2566,7 +2627,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>75</v>
       </c>
@@ -2586,7 +2647,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -2606,7 +2667,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -2626,7 +2687,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -2646,7 +2707,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -2666,7 +2727,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>139</v>
       </c>
@@ -2686,7 +2747,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>139</v>
       </c>
@@ -2706,32 +2767,32 @@
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="I16" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:9" x14ac:dyDescent="0.55000000000000004">
       <c r="I17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:9" x14ac:dyDescent="0.55000000000000004">
       <c r="I18" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:9" x14ac:dyDescent="0.55000000000000004">
       <c r="I19" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:9" x14ac:dyDescent="0.55000000000000004">
       <c r="I20" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:9" x14ac:dyDescent="0.55000000000000004">
       <c r="I21" t="s">
         <v>144</v>
       </c>
@@ -2742,23 +2803,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:O19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.15625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.26171875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>108</v>
       </c>
@@ -2775,7 +2836,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2792,7 +2853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2809,7 +2870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2826,7 +2887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2843,7 +2904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2860,7 +2921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2877,7 +2938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2894,7 +2955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2911,20 +2972,54 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>1</v>
-      </c>
-      <c r="B10" s="7" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10">
         <v>10</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" t="s">
         <v>194</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="6">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="6">
+        <v>11</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="6">
+        <v>1</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="6">
+        <v>12</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E12" s="6">
         <v>1</v>
       </c>
     </row>
@@ -2934,24 +3029,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.26171875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>106</v>
       </c>
@@ -2971,7 +3066,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="7" t="s">
         <v>187</v>
       </c>
@@ -2991,7 +3086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="7" t="s">
         <v>187</v>
       </c>
@@ -3011,7 +3106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="7" t="s">
         <v>187</v>
       </c>
@@ -3031,7 +3126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="7" t="s">
         <v>187</v>
       </c>
@@ -3051,7 +3146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -3071,7 +3166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -3091,7 +3186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>75</v>
       </c>
@@ -3111,7 +3206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>173</v>
       </c>
@@ -3131,7 +3226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>173</v>
       </c>
@@ -3151,7 +3246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>175</v>
       </c>
@@ -3171,7 +3266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>175</v>
       </c>
@@ -3191,7 +3286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>129</v>
       </c>
@@ -3211,7 +3306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>129</v>
       </c>
@@ -3231,7 +3326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>129</v>
       </c>
@@ -3251,7 +3346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>129</v>
       </c>
@@ -3271,7 +3366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -3291,7 +3386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>139</v>
       </c>
@@ -3311,7 +3406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="7" t="s">
         <v>191</v>
       </c>
@@ -3331,7 +3426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="7" t="s">
         <v>191</v>
       </c>
@@ -3351,7 +3446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="7" t="s">
         <v>191</v>
       </c>
@@ -3371,7 +3466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="7" t="s">
         <v>191</v>
       </c>
@@ -3391,7 +3486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>177</v>
       </c>
@@ -3411,7 +3506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>177</v>
       </c>
@@ -3431,7 +3526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>179</v>
       </c>
@@ -3451,7 +3546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>179</v>
       </c>
@@ -3471,7 +3566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>181</v>
       </c>
@@ -3491,7 +3586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>181</v>
       </c>
@@ -3511,7 +3606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -3531,7 +3626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>183</v>
       </c>
@@ -3551,7 +3646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>183</v>
       </c>
@@ -3571,7 +3666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>183</v>
       </c>
@@ -3591,7 +3686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>183</v>
       </c>
@@ -3617,19 +3712,19 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.15625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -3640,7 +3735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3651,7 +3746,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3662,7 +3757,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3673,7 +3768,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -3684,7 +3779,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -3695,7 +3790,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -3706,7 +3801,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -3717,7 +3812,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -3728,7 +3823,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -3739,7 +3834,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -3750,7 +3845,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -3761,7 +3856,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -3772,7 +3867,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -3783,7 +3878,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -3794,7 +3889,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -3805,7 +3900,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -3816,7 +3911,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -3827,7 +3922,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -3838,7 +3933,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -3849,7 +3944,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -3860,7 +3955,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -3871,7 +3966,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -3882,7 +3977,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -3893,7 +3988,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -3904,7 +3999,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -3915,7 +4010,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -3926,7 +4021,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -3937,7 +4032,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -3948,7 +4043,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -3959,7 +4054,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -3970,7 +4065,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -3981,7 +4076,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -3992,7 +4087,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -4003,7 +4098,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -4014,7 +4109,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -4025,7 +4120,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -4036,7 +4131,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -4047,7 +4142,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -4058,7 +4153,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>1</v>
       </c>
@@ -4069,7 +4164,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>1</v>
       </c>
@@ -4080,7 +4175,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>1</v>
       </c>
@@ -4091,7 +4186,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>1</v>
       </c>
@@ -4102,7 +4197,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>1</v>
       </c>
@@ -4113,7 +4208,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>1</v>
       </c>
@@ -4124,7 +4219,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -4135,7 +4230,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>1</v>
       </c>
@@ -4146,7 +4241,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
TFS 23919 - Allow Training Managers to Reassign CSR Module logs in Admin Tool
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C51098
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OmniCloud\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40A8249-9ABC-4041-B641-89E0E79C0050}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A080E74-70E7-4B82-B4D6-12D1BB2E273F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="596" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="AT_Entitlement" sheetId="23" r:id="rId3"/>
     <sheet name="AT_Role_Entitlement_Link" sheetId="28" r:id="rId4"/>
     <sheet name="AT_Action_Reasons" sheetId="24" r:id="rId5"/>
-    <sheet name="AT_Module_Access" sheetId="25" state="hidden" r:id="rId6"/>
+    <sheet name="AT_Module_Access" sheetId="25" r:id="rId6"/>
     <sheet name="AT_Reassign_Status_For_Module" sheetId="26" r:id="rId7"/>
     <sheet name="AT_Role_Access" sheetId="27" r:id="rId8"/>
     <sheet name="Historical_Source" sheetId="6" state="hidden" r:id="rId9"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="202">
   <si>
     <t>SourceID</t>
   </si>
@@ -465,9 +465,6 @@
     <t xml:space="preserve">           ('WPPM50','Manager, Program',1,'CSR',1),</t>
   </si>
   <si>
-    <t xml:space="preserve">          ('WPPM50','Manager, Program',2,'Supervisor',1) </t>
-  </si>
-  <si>
     <t>Sr Analyst, Functional</t>
   </si>
   <si>
@@ -631,6 +628,15 @@
   </si>
   <si>
     <t>Pending Follow-up Coaching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          ('WPPM50','Manager, Program',2,'Supervisor',1) ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WTTR50','Manager, Training',1,'CSR',1)</t>
+  </si>
+  <si>
+    <t>Allow Training Managers to Reassign CSR Module logs. Added row in AT_Module_Access tab</t>
   </si>
 </sst>
 </file>
@@ -692,7 +698,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -701,7 +707,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1041,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1189,7 +1194,7 @@
         <v>6246</v>
       </c>
       <c r="E8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1206,7 +1211,7 @@
         <v>5420</v>
       </c>
       <c r="E9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1214,7 +1219,7 @@
         <v>5641</v>
       </c>
       <c r="E10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1222,7 +1227,7 @@
         <v>5642</v>
       </c>
       <c r="E11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1239,7 +1244,7 @@
         <v>6591</v>
       </c>
       <c r="E12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1256,7 +1261,7 @@
         <v>8363</v>
       </c>
       <c r="E13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1273,14 +1278,14 @@
         <v>10823</v>
       </c>
       <c r="E14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7">
         <v>11</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="8">
         <v>43402</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -1290,14 +1295,14 @@
         <v>12473</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="7">
         <v>12</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="8">
         <v>43560</v>
       </c>
       <c r="C16" s="7" t="s">
@@ -1307,14 +1312,14 @@
         <v>13333</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="7">
         <v>13</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="8">
         <v>43714</v>
       </c>
       <c r="C17" s="7" t="s">
@@ -1324,14 +1329,14 @@
         <v>13644</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="7">
         <v>14</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="8">
         <v>44049</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1341,24 +1346,41 @@
         <v>18019</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="6">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="7">
         <v>15</v>
       </c>
       <c r="B19" s="8">
         <v>44454</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="7">
         <v>22187</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>197</v>
+      <c r="E19" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="7">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1">
+        <v>44587</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="7">
+        <v>23919</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -1442,7 +1464,7 @@
         <v>106</v>
       </c>
       <c r="B6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1453,7 +1475,7 @@
         <v>107</v>
       </c>
       <c r="B7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1464,7 +1486,7 @@
         <v>108</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1475,7 +1497,7 @@
         <v>109</v>
       </c>
       <c r="B9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1486,7 +1508,7 @@
         <v>110</v>
       </c>
       <c r="B10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1497,7 +1519,7 @@
         <v>111</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1508,7 +1530,7 @@
         <v>112</v>
       </c>
       <c r="B12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1519,7 +1541,7 @@
         <v>113</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1530,7 +1552,7 @@
         <v>114</v>
       </c>
       <c r="B14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1541,7 +1563,7 @@
         <v>115</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1552,7 +1574,7 @@
         <v>116</v>
       </c>
       <c r="B16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1563,7 +1585,7 @@
         <v>117</v>
       </c>
       <c r="B17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1574,7 +1596,7 @@
         <v>118</v>
       </c>
       <c r="B18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1585,7 +1607,7 @@
         <v>119</v>
       </c>
       <c r="B19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1683,7 +1705,7 @@
         <v>209</v>
       </c>
       <c r="B9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1691,7 +1713,7 @@
         <v>210</v>
       </c>
       <c r="B10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1699,7 +1721,7 @@
         <v>211</v>
       </c>
       <c r="B11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1707,7 +1729,7 @@
         <v>212</v>
       </c>
       <c r="B12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1715,7 +1737,7 @@
         <v>213</v>
       </c>
       <c r="B13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1723,7 +1745,7 @@
         <v>214</v>
       </c>
       <c r="B14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1731,7 +1753,7 @@
         <v>215</v>
       </c>
       <c r="B15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1739,7 +1761,7 @@
         <v>216</v>
       </c>
       <c r="B16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1747,7 +1769,7 @@
         <v>217</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2451,10 +2473,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2464,7 +2486,7 @@
     <col min="3" max="3" width="9.578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.41796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="101.41796875" customWidth="1"/>
+    <col min="9" max="9" width="101.41796875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2768,6 +2790,21 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="6">
+        <v>1</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1</v>
+      </c>
       <c r="I16" t="s">
         <v>141</v>
       </c>
@@ -2794,7 +2831,12 @@
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.55000000000000004">
       <c r="I21" t="s">
-        <v>144</v>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="I22" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2806,8 +2848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2983,43 +3025,43 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="6">
-        <v>1</v>
-      </c>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="7">
+        <v>1</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="7">
         <v>11</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E11" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="7">
+        <v>1</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="7">
+        <v>12</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="E11" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="6">
-        <v>1</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="6">
-        <v>12</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="E12" s="6">
+      <c r="E12" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3032,7 +3074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
@@ -3068,10 +3110,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>187</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>188</v>
       </c>
       <c r="C2">
         <v>101</v>
@@ -3088,10 +3130,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>187</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>188</v>
       </c>
       <c r="C3">
         <v>103</v>
@@ -3108,16 +3150,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>187</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>188</v>
       </c>
       <c r="C4">
         <v>106</v>
       </c>
       <c r="D4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -3128,16 +3170,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>187</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>188</v>
       </c>
       <c r="C5">
         <v>107</v>
       </c>
       <c r="D5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3208,16 +3250,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B9" t="s">
         <v>173</v>
-      </c>
-      <c r="B9" t="s">
-        <v>174</v>
       </c>
       <c r="C9">
         <v>106</v>
       </c>
       <c r="D9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -3228,16 +3270,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B10" t="s">
         <v>173</v>
-      </c>
-      <c r="B10" t="s">
-        <v>174</v>
       </c>
       <c r="C10">
         <v>107</v>
       </c>
       <c r="D10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -3248,16 +3290,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
+        <v>174</v>
+      </c>
+      <c r="B11" t="s">
         <v>175</v>
-      </c>
-      <c r="B11" t="s">
-        <v>176</v>
       </c>
       <c r="C11">
         <v>106</v>
       </c>
       <c r="D11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -3268,16 +3310,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
+        <v>174</v>
+      </c>
+      <c r="B12" t="s">
         <v>175</v>
-      </c>
-      <c r="B12" t="s">
-        <v>176</v>
       </c>
       <c r="C12">
         <v>107</v>
       </c>
       <c r="D12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -3317,7 +3359,7 @@
         <v>106</v>
       </c>
       <c r="D14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -3337,7 +3379,7 @@
         <v>107</v>
       </c>
       <c r="D15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -3408,10 +3450,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C19" s="7">
         <v>101</v>
@@ -3428,10 +3470,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C20" s="7">
         <v>103</v>
@@ -3448,16 +3490,16 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C21" s="7">
         <v>106</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E21" s="7">
         <v>0</v>
@@ -3468,16 +3510,16 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C22" s="7">
         <v>107</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E22" s="7">
         <v>0</v>
@@ -3488,16 +3530,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
+        <v>176</v>
+      </c>
+      <c r="B23" t="s">
         <v>177</v>
-      </c>
-      <c r="B23" t="s">
-        <v>178</v>
       </c>
       <c r="C23">
         <v>106</v>
       </c>
       <c r="D23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -3508,16 +3550,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
+        <v>176</v>
+      </c>
+      <c r="B24" t="s">
         <v>177</v>
-      </c>
-      <c r="B24" t="s">
-        <v>178</v>
       </c>
       <c r="C24">
         <v>107</v>
       </c>
       <c r="D24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -3528,16 +3570,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
+        <v>178</v>
+      </c>
+      <c r="B25" t="s">
         <v>179</v>
-      </c>
-      <c r="B25" t="s">
-        <v>180</v>
       </c>
       <c r="C25">
         <v>106</v>
       </c>
       <c r="D25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -3548,16 +3590,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
+        <v>178</v>
+      </c>
+      <c r="B26" t="s">
         <v>179</v>
-      </c>
-      <c r="B26" t="s">
-        <v>180</v>
       </c>
       <c r="C26">
         <v>107</v>
       </c>
       <c r="D26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -3568,16 +3610,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
+        <v>180</v>
+      </c>
+      <c r="B27" t="s">
         <v>181</v>
-      </c>
-      <c r="B27" t="s">
-        <v>182</v>
       </c>
       <c r="C27">
         <v>106</v>
       </c>
       <c r="D27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -3588,16 +3630,16 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
+        <v>180</v>
+      </c>
+      <c r="B28" t="s">
         <v>181</v>
-      </c>
-      <c r="B28" t="s">
-        <v>182</v>
       </c>
       <c r="C28">
         <v>107</v>
       </c>
       <c r="D28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -3628,10 +3670,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
+        <v>182</v>
+      </c>
+      <c r="B30" t="s">
         <v>183</v>
-      </c>
-      <c r="B30" t="s">
-        <v>184</v>
       </c>
       <c r="C30">
         <v>101</v>
@@ -3648,10 +3690,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
+        <v>182</v>
+      </c>
+      <c r="B31" t="s">
         <v>183</v>
-      </c>
-      <c r="B31" t="s">
-        <v>184</v>
       </c>
       <c r="C31">
         <v>103</v>
@@ -3668,16 +3710,16 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
+        <v>182</v>
+      </c>
+      <c r="B32" t="s">
         <v>183</v>
-      </c>
-      <c r="B32" t="s">
-        <v>184</v>
       </c>
       <c r="C32">
         <v>106</v>
       </c>
       <c r="D32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -3688,16 +3730,16 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
+        <v>182</v>
+      </c>
+      <c r="B33" t="s">
         <v>183</v>
-      </c>
-      <c r="B33" t="s">
-        <v>184</v>
       </c>
       <c r="C33">
         <v>107</v>
       </c>
       <c r="D33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E33">
         <v>0</v>

</xml_diff>

<commit_message>
TFS 24924 - Report access for Early Work Life Supervisors
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C51786
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OmniCloud\eCoaching_V2\Design\DD\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A080E74-70E7-4B82-B4D6-12D1BB2E273F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1490310-9B01-49C7-8A6E-C05F5E500EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" tabRatio="596" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -24,14 +24,14 @@
     <sheet name="Historical_Source" sheetId="6" state="hidden" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">AT_Role_Entitlement_Link!$A$1:$A$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">AT_Role_Entitlement_Link!$A$1:$A$51</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="205">
   <si>
     <t>SourceID</t>
   </si>
@@ -637,6 +637,15 @@
   </si>
   <si>
     <t>Allow Training Managers to Reassign CSR Module logs. Added row in AT_Module_Access tab</t>
+  </si>
+  <si>
+    <t>Report access for Early Work Life Supervisors. Added rows in Tables AT_Module_Access, AT_Role_Access, AT_Role_Entitlement_Link</t>
+  </si>
+  <si>
+    <t>WACS40</t>
+  </si>
+  <si>
+    <t>Supervisor, Customer Service</t>
   </si>
 </sst>
 </file>
@@ -698,7 +707,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -708,6 +717,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1046,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1381,6 +1392,20 @@
       </c>
       <c r="E20" s="7" t="s">
         <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="10">
+        <v>44762</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="6">
+        <v>24924</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -1779,10 +1804,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="A22" sqref="A22:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1962,11 +1987,11 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22">
-        <v>109</v>
-      </c>
-      <c r="B22">
-        <v>209</v>
+      <c r="A22" s="6">
+        <v>108</v>
+      </c>
+      <c r="B22" s="6">
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1974,15 +1999,15 @@
         <v>109</v>
       </c>
       <c r="B23">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B24">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1990,15 +2015,15 @@
         <v>110</v>
       </c>
       <c r="B25">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B26">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2006,15 +2031,15 @@
         <v>111</v>
       </c>
       <c r="B27">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B28">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2022,15 +2047,15 @@
         <v>112</v>
       </c>
       <c r="B29">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B30">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2038,15 +2063,15 @@
         <v>113</v>
       </c>
       <c r="B31">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B32">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2054,15 +2079,15 @@
         <v>114</v>
       </c>
       <c r="B33">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B34">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2070,15 +2095,15 @@
         <v>115</v>
       </c>
       <c r="B35">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B36">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2086,15 +2111,15 @@
         <v>116</v>
       </c>
       <c r="B37">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B38">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2102,63 +2127,63 @@
         <v>117</v>
       </c>
       <c r="B39">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B40">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B41">
-        <v>215</v>
-      </c>
-      <c r="F41" s="3"/>
+        <v>214</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>119</v>
       </c>
       <c r="B42">
+        <v>215</v>
+      </c>
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
+        <v>119</v>
+      </c>
+      <c r="B43">
         <v>216</v>
       </c>
-      <c r="F42" s="3"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="7">
-        <v>106</v>
-      </c>
-      <c r="B43" s="7">
-        <v>217</v>
-      </c>
+      <c r="F43" s="3"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="7">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B44" s="7">
         <v>217</v>
       </c>
-      <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="7">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B45" s="7">
         <v>217</v>
       </c>
+      <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="7">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B46" s="7">
         <v>217</v>
@@ -2166,7 +2191,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="7">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B47" s="7">
         <v>217</v>
@@ -2174,14 +2199,22 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="7">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B48" s="7">
         <v>217</v>
       </c>
     </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="7">
+        <v>116</v>
+      </c>
+      <c r="B49" s="7">
+        <v>217</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:A50" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
+  <autoFilter ref="A1:A51" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -2476,7 +2509,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2790,51 +2823,66 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="6">
-        <v>1</v>
-      </c>
-      <c r="D16" s="6" t="s">
+      <c r="C16" s="9">
+        <v>1</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="9">
         <v>1</v>
       </c>
       <c r="I16" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="6">
+        <v>1</v>
+      </c>
       <c r="I17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="I18" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="I19" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="I20" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="I21" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="I22" t="s">
         <v>200</v>
       </c>
@@ -3072,10 +3120,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3745,6 +3793,66 @@
         <v>0</v>
       </c>
       <c r="F33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C34" s="6">
+        <v>108</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E34" s="6">
+        <v>0</v>
+      </c>
+      <c r="F34" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="6">
+        <v>108</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E35" s="6">
+        <v>0</v>
+      </c>
+      <c r="F35" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="6">
+        <v>108</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E36" s="6">
+        <v>0</v>
+      </c>
+      <c r="F36" s="6">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TFS 25961- Update Manager permissions to reactivate Coaching Logs
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C52332
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1490310-9B01-49C7-8A6E-C05F5E500EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB8A726-04F7-4911-8CA3-32DEC386422B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" tabRatio="596" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57504" yWindow="1932" windowWidth="28992" windowHeight="15792" tabRatio="596" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -24,14 +24,14 @@
     <sheet name="Historical_Source" sheetId="6" state="hidden" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">AT_Role_Entitlement_Link!$A$1:$A$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">AT_Role_Entitlement_Link!$A$1:$A$3</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="206">
   <si>
     <t>SourceID</t>
   </si>
@@ -646,6 +646,9 @@
   </si>
   <si>
     <t>Supervisor, Customer Service</t>
+  </si>
+  <si>
+    <t>Update Manager permissions to reactivate Coaching Logs. Updated tab AT_Role_Entitlement_Link</t>
   </si>
 </sst>
 </file>
@@ -707,13 +710,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1057,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:E21"/>
+      <selection activeCell="B22" sqref="B22:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1292,120 +1292,134 @@
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="7">
+    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="4">
         <v>11</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="5">
         <v>43402</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="4">
         <v>12473</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="4" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="7">
+      <c r="A16" s="4">
         <v>12</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="5">
         <v>43560</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="4">
         <v>13333</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="4" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="7">
+      <c r="A17" s="4">
         <v>13</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="5">
         <v>43714</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="4">
         <v>13644</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="4" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="7">
+    <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="4">
         <v>14</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="5">
         <v>44049</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="4">
         <v>18019</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="4" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="7">
+    <row r="19" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="4">
         <v>15</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="5">
         <v>44454</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="4">
         <v>22187</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="4" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="7">
+      <c r="A20" s="4">
         <v>1</v>
       </c>
       <c r="B20" s="1">
         <v>44587</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="4">
         <v>23919</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="4" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="10">
+      <c r="B21" s="5">
         <v>44762</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="4">
         <v>24924</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="4" t="s">
         <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="7">
+        <v>44914</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="3">
+        <v>25961</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -1790,10 +1804,10 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="7">
+      <c r="A17" s="4">
         <v>217</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="4" t="s">
         <v>192</v>
       </c>
     </row>
@@ -1804,10 +1818,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1817,7 +1831,7 @@
     <col min="6" max="6" width="62.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>79</v>
       </c>
@@ -1825,7 +1839,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>101</v>
       </c>
@@ -1833,7 +1847,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>101</v>
       </c>
@@ -1841,7 +1855,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>101</v>
       </c>
@@ -1849,7 +1863,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>101</v>
       </c>
@@ -1857,7 +1871,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>101</v>
       </c>
@@ -1865,7 +1879,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>102</v>
       </c>
@@ -1873,7 +1887,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>102</v>
       </c>
@@ -1881,69 +1895,68 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="3">
         <v>102</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>102</v>
+      </c>
+      <c r="B10">
         <v>204</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
-        <v>103</v>
-      </c>
-      <c r="B10">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11">
-        <v>103</v>
-      </c>
-      <c r="B11">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="3">
+        <v>102</v>
+      </c>
+      <c r="B11" s="3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>103</v>
       </c>
       <c r="B12">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>103</v>
       </c>
       <c r="B13">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>103</v>
+      </c>
+      <c r="B14">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>103</v>
+      </c>
+      <c r="B15">
         <v>207</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14">
-        <v>106</v>
-      </c>
-      <c r="B14">
-        <v>209</v>
-      </c>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15">
-        <v>106</v>
-      </c>
-      <c r="B15">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>106</v>
       </c>
       <c r="B16">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1951,52 +1964,52 @@
         <v>106</v>
       </c>
       <c r="B17">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B18">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B19">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B20">
-        <v>209</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B21">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="6">
-        <v>108</v>
-      </c>
-      <c r="B22" s="6">
+      <c r="A22">
+        <v>107</v>
+      </c>
+      <c r="B22">
         <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B23">
         <v>209</v>
@@ -2004,63 +2017,63 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B24">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B25">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B26">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B27">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B28">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B29">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B30">
-        <v>210</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B31">
         <v>209</v>
@@ -2068,153 +2081,157 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B32">
         <v>211</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B33">
         <v>209</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B34">
         <v>210</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
+        <v>112</v>
+      </c>
+      <c r="B35">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>113</v>
+      </c>
+      <c r="B36">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>113</v>
+      </c>
+      <c r="B37">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>114</v>
+      </c>
+      <c r="B38">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>114</v>
+      </c>
+      <c r="B39">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>114</v>
+      </c>
+      <c r="B40">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
         <v>115</v>
       </c>
-      <c r="B35">
+      <c r="B41">
         <v>209</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42">
         <v>115</v>
       </c>
-      <c r="B36">
+      <c r="B42">
         <v>211</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
         <v>116</v>
       </c>
-      <c r="B37">
+      <c r="B43">
         <v>209</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44">
         <v>116</v>
       </c>
-      <c r="B38">
+      <c r="B44">
         <v>210</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45">
+        <v>116</v>
+      </c>
+      <c r="B45">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46">
         <v>117</v>
       </c>
-      <c r="B39">
+      <c r="B46">
         <v>209</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47">
         <v>117</v>
       </c>
-      <c r="B40">
+      <c r="B47">
         <v>211</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48">
         <v>118</v>
       </c>
-      <c r="B41">
+      <c r="B48">
         <v>214</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49">
         <v>119</v>
       </c>
-      <c r="B42">
+      <c r="B49">
         <v>215</v>
       </c>
-      <c r="F42" s="3"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
         <v>119</v>
       </c>
-      <c r="B43">
+      <c r="B50">
         <v>216</v>
       </c>
-      <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="7">
-        <v>106</v>
-      </c>
-      <c r="B44" s="7">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="7">
-        <v>108</v>
-      </c>
-      <c r="B45" s="7">
-        <v>217</v>
-      </c>
-      <c r="F45" s="5"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="7">
-        <v>110</v>
-      </c>
-      <c r="B46" s="7">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="7">
-        <v>112</v>
-      </c>
-      <c r="B47" s="7">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="7">
-        <v>114</v>
-      </c>
-      <c r="B48" s="7">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="7">
-        <v>116</v>
-      </c>
-      <c r="B49" s="7">
-        <v>217</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A51" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -2823,19 +2840,19 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="9">
-        <v>1</v>
-      </c>
-      <c r="D16" s="9" t="s">
+      <c r="C16" s="6">
+        <v>1</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="6">
         <v>1</v>
       </c>
       <c r="I16" t="s">
@@ -2843,19 +2860,19 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C17" s="6">
-        <v>1</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="3">
         <v>1</v>
       </c>
       <c r="I17" t="s">
@@ -3080,36 +3097,36 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="7">
-        <v>1</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="4">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="4">
         <v>11</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="7">
-        <v>1</v>
-      </c>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="4">
+        <v>1</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="4">
         <v>12</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3122,7 +3139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
@@ -3157,10 +3174,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>187</v>
       </c>
       <c r="C2">
@@ -3177,10 +3194,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>187</v>
       </c>
       <c r="C3">
@@ -3197,10 +3214,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>187</v>
       </c>
       <c r="C4">
@@ -3217,10 +3234,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>187</v>
       </c>
       <c r="C5">
@@ -3497,82 +3514,82 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="4">
         <v>101</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="7">
-        <v>0</v>
-      </c>
-      <c r="F19" s="7">
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="4">
         <v>103</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="7">
-        <v>0</v>
-      </c>
-      <c r="F20" s="7">
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="4">
         <v>106</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E21" s="7">
-        <v>0</v>
-      </c>
-      <c r="F21" s="7">
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="4">
         <v>107</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="E22" s="7">
-        <v>0</v>
-      </c>
-      <c r="F22" s="7">
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3797,62 +3814,62 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="3">
         <v>108</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="E34" s="6">
-        <v>0</v>
-      </c>
-      <c r="F34" s="6">
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="3">
         <v>108</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="E35" s="6">
-        <v>0</v>
-      </c>
-      <c r="F35" s="6">
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="3">
         <v>108</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="E36" s="6">
-        <v>0</v>
-      </c>
-      <c r="F36" s="6">
+      <c r="E36" s="3">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TFS 27527 - Create eCoaching Log for Subcontractors
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C53615
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB8A726-04F7-4911-8CA3-32DEC386422B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631AF0C7-2C23-4609-962F-E199E0498098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57504" yWindow="1932" windowWidth="28992" windowHeight="15792" tabRatio="596" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" tabRatio="596" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="208">
   <si>
     <t>SourceID</t>
   </si>
@@ -649,6 +649,12 @@
   </si>
   <si>
     <t>Update Manager permissions to reactivate Coaching Logs. Updated tab AT_Role_Entitlement_Link</t>
+  </si>
+  <si>
+    <t>Create eCoaching Log for Subcontractors</t>
+  </si>
+  <si>
+    <t>SubAdmin</t>
   </si>
 </sst>
 </file>
@@ -710,7 +716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -719,6 +725,7 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,9 +744,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -777,9 +784,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -812,26 +819,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -864,26 +854,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1057,10 +1030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1379,7 +1352,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1">
         <v>44587</v>
@@ -1395,6 +1368,9 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="4">
+        <v>17</v>
+      </c>
       <c r="B21" s="5">
         <v>44762</v>
       </c>
@@ -1408,18 +1384,38 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B22" s="7">
+    <row r="22" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="6">
+        <v>18</v>
+      </c>
+      <c r="B22" s="8">
         <v>44914</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="6">
         <v>25961</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="6" t="s">
         <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="3">
+        <v>19</v>
+      </c>
+      <c r="B23" s="7">
+        <v>45356</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="3">
+        <v>27527</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1430,10 +1426,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1650,6 +1646,17 @@
       </c>
       <c r="C19">
         <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="3">
+        <v>120</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1818,10 +1825,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B11"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1896,26 +1903,26 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="3">
+      <c r="A9" s="6">
         <v>102</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="6">
         <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
+      <c r="A10" s="6">
         <v>102</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="6">
         <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="3">
+      <c r="A11" s="6">
         <v>102</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="6">
         <v>206</v>
       </c>
     </row>
@@ -2229,6 +2236,62 @@
       </c>
       <c r="B50">
         <v>216</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="3">
+        <v>120</v>
+      </c>
+      <c r="B51" s="3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="3">
+        <v>120</v>
+      </c>
+      <c r="B52" s="3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="3">
+        <v>120</v>
+      </c>
+      <c r="B53" s="3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="3">
+        <v>120</v>
+      </c>
+      <c r="B54" s="3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="3">
+        <v>120</v>
+      </c>
+      <c r="B55" s="3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="3">
+        <v>120</v>
+      </c>
+      <c r="B56" s="3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="3">
+        <v>120</v>
+      </c>
+      <c r="B57" s="3">
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 28026 - ISG Realignment Project
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C53863
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631AF0C7-2C23-4609-962F-E199E0498098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D0B58C-158F-4700-BB32-7DBD5B38B4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" tabRatio="596" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" tabRatio="596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -21,7 +21,8 @@
     <sheet name="AT_Module_Access" sheetId="25" r:id="rId6"/>
     <sheet name="AT_Reassign_Status_For_Module" sheetId="26" r:id="rId7"/>
     <sheet name="AT_Role_Access" sheetId="27" r:id="rId8"/>
-    <sheet name="Historical_Source" sheetId="6" state="hidden" r:id="rId9"/>
+    <sheet name="AT_Role_Module_Link" sheetId="29" r:id="rId9"/>
+    <sheet name="Historical_Source" sheetId="6" state="hidden" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">AT_Role_Entitlement_Link!$A$1:$A$3</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="210">
   <si>
     <t>SourceID</t>
   </si>
@@ -655,6 +656,12 @@
   </si>
   <si>
     <t>SubAdmin</t>
+  </si>
+  <si>
+    <t>ISG</t>
+  </si>
+  <si>
+    <t>ISG Realignment Project. Added rows or columns in tabs AT_Module_Access, AT_Reassign_Status_For_Module, AT_Role_Module_Link</t>
   </si>
 </sst>
 </file>
@@ -724,8 +731,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1030,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:E23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1299,7 +1306,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4">
         <v>13</v>
       </c>
@@ -1316,7 +1323,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="4">
         <v>14</v>
       </c>
@@ -1333,7 +1340,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4">
         <v>15</v>
       </c>
@@ -1350,7 +1357,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4">
         <v>16</v>
       </c>
@@ -1367,7 +1374,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4">
         <v>17</v>
       </c>
@@ -1384,11 +1391,11 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="6">
         <v>18</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="7">
         <v>44914</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -1401,26 +1408,590 @@
         <v>205</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="4">
         <v>19</v>
       </c>
-      <c r="B23" s="7">
-        <v>45356</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="B23" s="1">
+        <v>45376</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="4">
         <v>27527</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="4" t="s">
         <v>206</v>
+      </c>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="3">
+        <v>20</v>
+      </c>
+      <c r="B24" s="8">
+        <v>45432</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="3">
+        <v>28026</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:C48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="12.15625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C44">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48">
+        <v>208</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1428,7 +1999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20:C20"/>
     </sheetView>
   </sheetViews>
@@ -1649,13 +2220,13 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="3">
+      <c r="A20" s="4">
         <v>120</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2239,58 +2810,58 @@
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="3">
+      <c r="A51" s="4">
         <v>120</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="4">
         <v>201</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="3">
+      <c r="A52" s="4">
         <v>120</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="4">
         <v>202</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="3">
+      <c r="A53" s="4">
         <v>120</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="4">
         <v>203</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="3">
+      <c r="A54" s="4">
         <v>120</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="4">
         <v>204</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="3">
+      <c r="A55" s="4">
         <v>120</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B55" s="4">
         <v>205</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="3">
+      <c r="A56" s="4">
         <v>120</v>
       </c>
-      <c r="B56" s="3">
+      <c r="B56" s="4">
         <v>206</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="3">
+      <c r="A57" s="4">
         <v>120</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B57" s="4">
         <v>207</v>
       </c>
     </row>
@@ -2586,10 +3157,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+      <selection activeCell="A18" sqref="A18:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2923,19 +3494,19 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="C17" s="3">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="C17" s="4">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="4">
         <v>1</v>
       </c>
       <c r="I17" t="s">
@@ -2943,28 +3514,120 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" s="3">
+        <v>10</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
       <c r="I18" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="3">
+        <v>10</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
       <c r="I19" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="3">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
       <c r="I20" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C21" s="3">
+        <v>10</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
       <c r="I21" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="3">
+        <v>10</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
       <c r="I22" t="s">
         <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C23" s="3">
+        <v>10</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2974,10 +3637,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A13" sqref="A13:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3193,6 +3856,91 @@
         <v>1</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="3">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C13" s="3">
+        <v>5</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="3">
+        <v>10</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C14" s="3">
+        <v>6</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="3">
+        <v>10</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C15" s="3">
+        <v>10</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="3">
+        <v>10</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C16" s="3">
+        <v>11</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="3">
+        <v>10</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C17" s="3">
+        <v>12</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3203,7 +3951,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="A34" sqref="A34:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3877,62 +4625,62 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="4">
         <v>108</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E34" s="3">
-        <v>0</v>
-      </c>
-      <c r="F34" s="3">
+      <c r="E34" s="4">
+        <v>0</v>
+      </c>
+      <c r="F34" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="4">
         <v>108</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E35" s="3">
-        <v>0</v>
-      </c>
-      <c r="F35" s="3">
+      <c r="E35" s="4">
+        <v>0</v>
+      </c>
+      <c r="F35" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="4">
         <v>108</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E36" s="3">
-        <v>0</v>
-      </c>
-      <c r="F36" s="3">
+      <c r="E36" s="4">
+        <v>0</v>
+      </c>
+      <c r="F36" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3942,544 +4690,213 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB89CA7B-9E7C-4D87-AB15-9C2BA04A5FA1}">
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:B25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="12.15625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83984375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>106</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>106</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>106</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>106</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>106</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>107</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>107</v>
+      </c>
+      <c r="B8">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>107</v>
+      </c>
+      <c r="B9">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>107</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>107</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>108</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>109</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>110</v>
+      </c>
+      <c r="B14">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>111</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>112</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>113</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>114</v>
+      </c>
+      <c r="B18">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>115</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>116</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>117</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="3">
+        <v>106</v>
+      </c>
+      <c r="B22" s="3">
         <v>10</v>
       </c>
-      <c r="C17">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" t="s">
-        <v>49</v>
-      </c>
-      <c r="C35">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" t="s">
-        <v>19</v>
-      </c>
-      <c r="C39">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
-        <v>20</v>
-      </c>
-      <c r="C40">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" t="s">
-        <v>21</v>
-      </c>
-      <c r="C41">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B42" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" t="s">
-        <v>1</v>
-      </c>
-      <c r="B44" t="s">
-        <v>27</v>
-      </c>
-      <c r="C44">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" t="s">
-        <v>1</v>
-      </c>
-      <c r="B45" t="s">
-        <v>28</v>
-      </c>
-      <c r="C45">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46" t="s">
-        <v>29</v>
-      </c>
-      <c r="C46">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" t="s">
-        <v>1</v>
-      </c>
-      <c r="B47" t="s">
-        <v>52</v>
-      </c>
-      <c r="C47">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" t="s">
-        <v>1</v>
-      </c>
-      <c r="B48" t="s">
-        <v>6</v>
-      </c>
-      <c r="C48">
-        <v>208</v>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="3">
+        <v>107</v>
+      </c>
+      <c r="B23" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="3">
+        <v>108</v>
+      </c>
+      <c r="B24" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="3">
+        <v>109</v>
+      </c>
+      <c r="B25" s="3">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TFS 28361 - Add the Production Planning Module to eCoaching
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C54160
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_Log_AT_Dimension_Table_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D0B58C-158F-4700-BB32-7DBD5B38B4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16685F9-46BA-4163-B9B7-CFF289040E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" tabRatio="596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57504" yWindow="1914" windowWidth="28992" windowHeight="15672" tabRatio="596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="215">
   <si>
     <t>SourceID</t>
   </si>
@@ -466,9 +466,6 @@
     <t xml:space="preserve">           ('WPPM50','Manager, Program',1,'CSR',1),</t>
   </si>
   <si>
-    <t>Sr Analyst, Functional</t>
-  </si>
-  <si>
     <t>Added rows for job code WPSM13 (Mark Hackman)AT_Role_Access tab</t>
   </si>
   <si>
@@ -662,6 +659,24 @@
   </si>
   <si>
     <t>ISG Realignment Project. Added rows or columns in tabs AT_Module_Access, AT_Reassign_Status_For_Module, AT_Role_Module_Link</t>
+  </si>
+  <si>
+    <t>WCWF50</t>
+  </si>
+  <si>
+    <t>Manager, WFM</t>
+  </si>
+  <si>
+    <t>Production Planning</t>
+  </si>
+  <si>
+    <t>WPOP60</t>
+  </si>
+  <si>
+    <t>Sr Manager, Operations</t>
+  </si>
+  <si>
+    <t>Production Planning Module. Added rows or columns in tabs AT_Module_Access, AT_Reassign_Status_For_Module, AT_Role_Access,  AT_Role_Module_Link</t>
   </si>
 </sst>
 </file>
@@ -1037,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1185,7 +1200,7 @@
         <v>6246</v>
       </c>
       <c r="E8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1202,7 +1217,7 @@
         <v>5420</v>
       </c>
       <c r="E9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1210,7 +1225,7 @@
         <v>5641</v>
       </c>
       <c r="E10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1218,7 +1233,7 @@
         <v>5642</v>
       </c>
       <c r="E11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1235,7 +1250,7 @@
         <v>6591</v>
       </c>
       <c r="E12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1252,7 +1267,7 @@
         <v>8363</v>
       </c>
       <c r="E13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1269,7 +1284,7 @@
         <v>10823</v>
       </c>
       <c r="E14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1286,7 +1301,7 @@
         <v>12473</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1303,7 +1318,7 @@
         <v>13333</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1320,7 +1335,7 @@
         <v>13644</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1337,7 +1352,7 @@
         <v>18019</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1354,7 +1369,7 @@
         <v>22187</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1371,7 +1386,7 @@
         <v>23919</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1388,7 +1403,7 @@
         <v>24924</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1405,7 +1420,7 @@
         <v>25961</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1422,25 +1437,42 @@
         <v>27527</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="3">
+      <c r="A24" s="4">
         <v>20</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="5">
         <v>45432</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="4">
         <v>28026</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>209</v>
+      <c r="E24" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="3">
+        <v>21</v>
+      </c>
+      <c r="B25" s="8">
+        <v>45530</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="3">
+        <v>28361</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -1999,9 +2031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:C20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -2070,7 +2100,7 @@
         <v>106</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2081,7 +2111,7 @@
         <v>107</v>
       </c>
       <c r="B7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2092,7 +2122,7 @@
         <v>108</v>
       </c>
       <c r="B8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -2103,7 +2133,7 @@
         <v>109</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -2114,7 +2144,7 @@
         <v>110</v>
       </c>
       <c r="B10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -2125,7 +2155,7 @@
         <v>111</v>
       </c>
       <c r="B11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -2136,7 +2166,7 @@
         <v>112</v>
       </c>
       <c r="B12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -2147,7 +2177,7 @@
         <v>113</v>
       </c>
       <c r="B13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -2158,7 +2188,7 @@
         <v>114</v>
       </c>
       <c r="B14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -2169,7 +2199,7 @@
         <v>115</v>
       </c>
       <c r="B15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -2180,7 +2210,7 @@
         <v>116</v>
       </c>
       <c r="B16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -2191,7 +2221,7 @@
         <v>117</v>
       </c>
       <c r="B17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -2202,7 +2232,7 @@
         <v>118</v>
       </c>
       <c r="B18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2213,7 +2243,7 @@
         <v>119</v>
       </c>
       <c r="B19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2224,7 +2254,7 @@
         <v>120</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C20" s="4">
         <v>0</v>
@@ -2239,9 +2269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -2322,7 +2350,7 @@
         <v>209</v>
       </c>
       <c r="B9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2330,7 +2358,7 @@
         <v>210</v>
       </c>
       <c r="B10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2338,7 +2366,7 @@
         <v>211</v>
       </c>
       <c r="B11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2346,7 +2374,7 @@
         <v>212</v>
       </c>
       <c r="B12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2354,7 +2382,7 @@
         <v>213</v>
       </c>
       <c r="B13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2362,7 +2390,7 @@
         <v>214</v>
       </c>
       <c r="B14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2370,7 +2398,7 @@
         <v>215</v>
       </c>
       <c r="B15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2378,7 +2406,7 @@
         <v>216</v>
       </c>
       <c r="B16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2386,7 +2414,7 @@
         <v>217</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2398,9 +2426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:B57"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -2875,9 +2901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -3157,10 +3181,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:E23"/>
+      <selection activeCell="A24" sqref="A24:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3495,10 +3519,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>204</v>
       </c>
       <c r="C17" s="4">
         <v>1</v>
@@ -3514,19 +3538,19 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="4">
         <v>10</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E18" s="3">
+      <c r="D18" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E18" s="4">
         <v>1</v>
       </c>
       <c r="I18" t="s">
@@ -3534,19 +3558,19 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="4">
         <v>10</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E19" s="3">
+      <c r="D19" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E19" s="4">
         <v>1</v>
       </c>
       <c r="I19" t="s">
@@ -3554,19 +3578,19 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="4">
         <v>10</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E20" s="3">
+      <c r="D20" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E20" s="4">
         <v>1</v>
       </c>
       <c r="I20" t="s">
@@ -3574,59 +3598,93 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="4">
         <v>10</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E21" s="3">
+      <c r="D21" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E21" s="4">
         <v>1</v>
       </c>
       <c r="I21" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="4">
+        <v>10</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="I22" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C23" s="4">
         <v>10</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E22" s="3">
-        <v>1</v>
-      </c>
-      <c r="I22" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C23" s="3">
-        <v>10</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E23" s="3">
+      <c r="D23" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C24" s="3">
+        <v>8</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C25" s="3">
+        <v>8</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E25" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3637,10 +3695,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:E17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3816,7 +3874,7 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -3833,7 +3891,7 @@
         <v>11</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E11" s="4">
         <v>1</v>
@@ -3850,94 +3908,128 @@
         <v>12</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E12" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="3">
+      <c r="A13" s="6">
         <v>10</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C13" s="3">
+      <c r="B13" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C13" s="6">
         <v>5</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="3">
+      <c r="A14" s="6">
         <v>10</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C14" s="3">
+      <c r="B14" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C14" s="6">
         <v>6</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="3">
+      <c r="A15" s="6">
         <v>10</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C15" s="3">
+      <c r="B15" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C15" s="6">
         <v>10</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="E15" s="3">
+      <c r="D15" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="E15" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="3">
+      <c r="A16" s="6">
         <v>10</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C16" s="3">
+      <c r="B16" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C16" s="6">
         <v>11</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="6">
+        <v>10</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C17" s="6">
+        <v>12</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="E16" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="3">
+      <c r="E17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="3">
+        <v>8</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C18" s="3">
+        <v>6</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="3">
+        <v>8</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C19" s="3">
         <v>10</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C17" s="3">
-        <v>12</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="E17" s="3">
+      <c r="D19" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E19" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3948,10 +4040,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:F36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3986,10 +4078,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
-        <v>186</v>
+        <v>129</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>187</v>
+        <v>136</v>
       </c>
       <c r="C2">
         <v>101</v>
@@ -4006,19 +4098,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
-        <v>186</v>
+        <v>59</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>187</v>
+        <v>60</v>
       </c>
       <c r="C3">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -4026,39 +4118,39 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
-        <v>186</v>
+        <v>61</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>187</v>
+        <v>62</v>
       </c>
       <c r="C4">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D4" t="s">
-        <v>149</v>
+        <v>83</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>187</v>
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>76</v>
       </c>
       <c r="C5">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>150</v>
+        <v>83</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -4066,10 +4158,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C6">
         <v>102</v>
@@ -4086,10 +4178,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C7">
         <v>102</v>
@@ -4106,19 +4198,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>136</v>
       </c>
       <c r="C8">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -4126,16 +4218,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="B9" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="C9">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D9" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -4146,16 +4238,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="B10" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="C10">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D10" t="s">
-        <v>150</v>
+        <v>84</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -4166,16 +4258,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
       <c r="B11" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
       <c r="C11">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -4186,19 +4278,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="B12" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="C12">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D12" t="s">
-        <v>150</v>
+        <v>83</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -4206,16 +4298,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>129</v>
+        <v>171</v>
       </c>
       <c r="B13" t="s">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="C13">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
+        <v>148</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -4226,13 +4318,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>129</v>
+        <v>171</v>
       </c>
       <c r="B14" t="s">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="C14">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D14" t="s">
         <v>149</v>
@@ -4246,16 +4338,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>173</v>
       </c>
       <c r="B15" t="s">
-        <v>136</v>
+        <v>174</v>
       </c>
       <c r="C15">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -4266,16 +4358,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>173</v>
       </c>
       <c r="B16" t="s">
-        <v>136</v>
+        <v>174</v>
       </c>
       <c r="C16">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D16" t="s">
-        <v>84</v>
+        <v>149</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -4286,56 +4378,56 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>175</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>176</v>
       </c>
       <c r="C17">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>148</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>139</v>
-      </c>
-      <c r="B18" t="s">
-        <v>140</v>
-      </c>
-      <c r="C18">
-        <v>102</v>
-      </c>
-      <c r="D18" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
+      <c r="A18" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C18" s="4">
+        <v>107</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="C19" s="4">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>82</v>
+        <v>148</v>
       </c>
       <c r="E19" s="4">
         <v>0</v>
@@ -4346,16 +4438,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="C20" s="4">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>84</v>
+        <v>149</v>
       </c>
       <c r="E20" s="4">
         <v>0</v>
@@ -4366,56 +4458,56 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4" t="s">
-        <v>190</v>
+        <v>129</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>189</v>
+        <v>136</v>
       </c>
       <c r="C21" s="4">
         <v>106</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>129</v>
+      </c>
+      <c r="B22" t="s">
+        <v>178</v>
+      </c>
+      <c r="C22">
+        <v>107</v>
+      </c>
+      <c r="D22" t="s">
         <v>149</v>
       </c>
-      <c r="E21" s="4">
-        <v>0</v>
-      </c>
-      <c r="F21" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="C22" s="4">
-        <v>107</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="E22" s="4">
-        <v>0</v>
-      </c>
-      <c r="F22" s="4">
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="B23" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="C23">
         <v>106</v>
       </c>
       <c r="D23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -4426,16 +4518,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="B24" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="C24">
         <v>107</v>
       </c>
       <c r="D24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -4446,16 +4538,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="B25" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="C25">
         <v>106</v>
       </c>
       <c r="D25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -4466,16 +4558,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="B26" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="C26">
         <v>107</v>
       </c>
       <c r="D26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -4486,16 +4578,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="B27" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="C27">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D27" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -4506,16 +4598,16 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="B28" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="C28">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D28" t="s">
-        <v>150</v>
+        <v>84</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -4526,19 +4618,19 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>179</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>180</v>
       </c>
       <c r="C29">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D29" t="s">
-        <v>83</v>
+        <v>148</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -4546,16 +4638,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B30" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C30">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D30" t="s">
-        <v>82</v>
+        <v>149</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -4566,16 +4658,16 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
+        <v>181</v>
+      </c>
+      <c r="B31" t="s">
         <v>182</v>
       </c>
-      <c r="B31" t="s">
-        <v>183</v>
-      </c>
       <c r="C31">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D31" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -4586,56 +4678,56 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
+        <v>181</v>
+      </c>
+      <c r="B32" t="s">
         <v>182</v>
       </c>
-      <c r="B32" t="s">
-        <v>183</v>
-      </c>
       <c r="C32">
+        <v>103</v>
+      </c>
+      <c r="D32" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C33" s="4">
         <v>106</v>
       </c>
-      <c r="D32" t="s">
-        <v>149</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" t="s">
-        <v>182</v>
-      </c>
-      <c r="B33" t="s">
-        <v>183</v>
-      </c>
-      <c r="C33">
-        <v>107</v>
-      </c>
-      <c r="D33" t="s">
-        <v>150</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
+      <c r="D33" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E33" s="4">
+        <v>0</v>
+      </c>
+      <c r="F33" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="4" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="C34" s="4">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E34" s="4">
         <v>0</v>
@@ -4655,7 +4747,7 @@
         <v>108</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E35" s="4">
         <v>0</v>
@@ -4665,22 +4757,62 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="4" t="s">
+      <c r="A36" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36">
         <v>108</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="E36" s="4">
-        <v>0</v>
-      </c>
-      <c r="F36" s="4">
+      <c r="D36" t="s">
+        <v>150</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C37" s="3">
+        <v>102</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E37" s="3">
+        <v>1</v>
+      </c>
+      <c r="F37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C38" s="3">
+        <v>102</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" s="3">
+        <v>1</v>
+      </c>
+      <c r="F38" s="3">
         <v>1</v>
       </c>
     </row>
@@ -4691,10 +4823,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB89CA7B-9E7C-4D87-AB15-9C2BA04A5FA1}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:B25"/>
+      <selection activeCell="A26" sqref="A26:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4868,35 +5000,43 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="3">
+      <c r="A22" s="4">
         <v>106</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="3">
+      <c r="A23" s="4">
         <v>107</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="3">
+      <c r="A24" s="4">
         <v>108</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="3">
+      <c r="A25" s="4">
         <v>109</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="4">
         <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="3">
+        <v>102</v>
+      </c>
+      <c r="B26" s="3">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>